<commit_message>
Version v1.3.0.0 - Modificada clase 'Facturas' para ajustar las propiedades y su orden segun campos obligatorios y opcionales - Modificado metodo 'Facturas.MapeoFacturas' para ajustar la numeracion de columnas segun propiedades de la clase - Modificado metodo 'ProcesoDiagram.EmitidasDiagram' para ajustar la carga de propiedades segun el mapeo de columnas - Creado metodo 'Utilidades.divideCadena' - Modificado metodo 'procesoAlcasal.emitidasAlcasal' para ajustar la carga de propiedades segun el mapeo de columnas - Creado metodo 'procesoAlcasal.MapeoColumnas' para la configuracion de las columnas a procesar y propiedades a exportar - Modificado metodo 'Procesos.leerExcel' para adaptar la lectura segun el mapeo de columnas - Creado metodo 'Procesos.LeerConfiguracionColumnas' para cargar el fichero de configuracion de columnas - Creado metodo 'Program.ProcesarArgumentos' para tratar los argumentos como parejas de 'clave=valor'
</commit_message>
<xml_diff>
--- a/pruebas/emitidasDiagram.xlsx
+++ b/pruebas/emitidasDiagram.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programacion\C#\importadorFacturas\pruebas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programacion\c#\importadorFacturas\pruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="180">
   <si>
     <t>Columna</t>
   </si>
@@ -507,36 +507,6 @@
     <t>05126963X</t>
   </si>
   <si>
-    <t>APELLIDO APELLIDO</t>
-  </si>
-  <si>
-    <t>NOMBRE</t>
-  </si>
-  <si>
-    <t>RODRIGUEZ SANCHEZ</t>
-  </si>
-  <si>
-    <t>REMEDIOS</t>
-  </si>
-  <si>
-    <t>ALBAPROA S.L.</t>
-  </si>
-  <si>
-    <t>CARLOS</t>
-  </si>
-  <si>
-    <t>CLEMENTE RODRIGUEZ</t>
-  </si>
-  <si>
-    <t>NARAJO RUIZ</t>
-  </si>
-  <si>
-    <t>M.JOSE</t>
-  </si>
-  <si>
-    <t>FRUTOS SECOS MANCHUELA</t>
-  </si>
-  <si>
     <t>DIRECCION CLIENTE 1</t>
   </si>
   <si>
@@ -577,6 +547,24 @@
   </si>
   <si>
     <t>Campos obligatorios</t>
+  </si>
+  <si>
+    <t>APELLIDO APELLIDO, NOMBRE</t>
+  </si>
+  <si>
+    <t>RODRIGUEZ SANCHEZ, REMEDIOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALBAPROA S.L., </t>
+  </si>
+  <si>
+    <t>CLEMENTE RODRIGUEZ, CARLOS</t>
+  </si>
+  <si>
+    <t>NARAJO RUIZ, M.JOSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FRUTOS SECOS MANCHUELA, </t>
   </si>
 </sst>
 </file>
@@ -604,7 +592,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -614,6 +602,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -728,7 +728,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -757,7 +757,12 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1040,1131 +1045,1106 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BM10"/>
+  <dimension ref="B1:BM10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AD3" sqref="AD3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.75" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.75" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.75" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="8" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="23.25" bestFit="1" customWidth="1"/>
-    <col min="31" max="32" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="17.375" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="14" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="19.625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="10" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="8.75" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="8.75" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="8.75" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="8.75" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="8.75" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.625" customWidth="1"/>
+    <col min="11" max="11" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="8" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="10.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65" x14ac:dyDescent="0.15">
-      <c r="A1" s="11">
+    <row r="1" spans="2:65" x14ac:dyDescent="0.15">
+      <c r="B1" s="11">
         <v>1</v>
       </c>
-      <c r="B1">
+      <c r="C1">
         <v>2</v>
       </c>
-      <c r="C1" s="11">
+      <c r="D1" s="11">
         <v>3</v>
       </c>
-      <c r="D1">
+      <c r="E1" s="11">
         <v>4</v>
       </c>
-      <c r="E1" s="11">
+      <c r="F1">
         <v>5</v>
       </c>
-      <c r="F1">
+      <c r="G1" s="11">
         <v>6</v>
       </c>
-      <c r="G1" s="11">
+      <c r="H1" s="11">
         <v>7</v>
       </c>
-      <c r="H1">
+      <c r="I1">
         <v>8</v>
       </c>
-      <c r="I1" s="11">
+      <c r="J1" s="11">
         <v>9</v>
       </c>
-      <c r="J1">
+      <c r="K1" s="11">
         <v>10</v>
       </c>
-      <c r="K1" s="11">
+      <c r="L1">
         <v>11</v>
       </c>
-      <c r="L1">
+      <c r="M1" s="11">
         <v>12</v>
       </c>
-      <c r="M1" s="11">
+      <c r="N1" s="11">
         <v>13</v>
       </c>
-      <c r="N1">
+      <c r="O1">
         <v>14</v>
       </c>
-      <c r="O1" s="11">
+      <c r="P1" s="11">
         <v>15</v>
       </c>
-      <c r="P1">
+      <c r="Q1" s="11">
         <v>16</v>
       </c>
-      <c r="Q1" s="11">
+      <c r="R1">
         <v>17</v>
       </c>
-      <c r="R1">
+      <c r="S1" s="11">
         <v>18</v>
       </c>
-      <c r="S1" s="11">
+      <c r="T1" s="11">
         <v>19</v>
       </c>
-      <c r="T1">
+      <c r="U1">
         <v>20</v>
       </c>
-      <c r="U1" s="11">
+      <c r="V1" s="11">
         <v>21</v>
       </c>
-      <c r="V1">
+      <c r="W1" s="11">
         <v>22</v>
       </c>
-      <c r="W1" s="11">
+      <c r="X1">
         <v>23</v>
       </c>
-      <c r="X1">
+      <c r="Y1" s="11">
         <v>24</v>
       </c>
-      <c r="Y1" s="11">
+      <c r="Z1" s="11">
         <v>25</v>
       </c>
-      <c r="Z1">
+      <c r="AA1">
         <v>26</v>
       </c>
-      <c r="AA1" s="11">
+      <c r="AB1" s="11">
         <v>27</v>
       </c>
-      <c r="AB1">
+      <c r="AC1" s="11">
         <v>28</v>
       </c>
-      <c r="AC1" s="11">
+      <c r="AD1">
         <v>29</v>
       </c>
-      <c r="AD1">
+      <c r="AE1" s="11">
         <v>30</v>
       </c>
-      <c r="AE1" s="11">
+      <c r="AF1" s="11">
         <v>31</v>
       </c>
-      <c r="AF1">
+      <c r="AG1">
         <v>32</v>
       </c>
-      <c r="AG1" s="11">
+      <c r="AH1" s="11">
         <v>33</v>
       </c>
-      <c r="AH1">
+      <c r="AI1" s="11">
         <v>34</v>
       </c>
-      <c r="AI1" s="11">
+      <c r="AJ1">
         <v>35</v>
       </c>
-      <c r="AJ1">
+      <c r="AK1" s="11">
         <v>36</v>
       </c>
-      <c r="AK1" s="11">
+      <c r="AL1" s="11">
         <v>37</v>
       </c>
-      <c r="AL1">
+      <c r="AM1">
         <v>38</v>
       </c>
-      <c r="AM1" s="11">
+      <c r="AN1" s="11">
         <v>39</v>
       </c>
-      <c r="AN1">
+      <c r="AO1" s="11">
         <v>40</v>
       </c>
-      <c r="AO1" s="11">
+      <c r="AP1">
         <v>41</v>
       </c>
-      <c r="AP1">
+      <c r="AQ1" s="11">
         <v>42</v>
       </c>
-      <c r="AQ1" s="11">
+      <c r="AR1" s="11">
         <v>43</v>
       </c>
-      <c r="AR1">
+      <c r="AS1">
         <v>44</v>
       </c>
-      <c r="AS1" s="11">
+      <c r="AT1" s="11">
         <v>45</v>
       </c>
-      <c r="AT1">
+      <c r="AU1" s="11">
         <v>46</v>
       </c>
-      <c r="AU1" s="11">
+      <c r="AV1">
         <v>47</v>
       </c>
-      <c r="AV1">
+      <c r="AW1" s="11">
         <v>48</v>
       </c>
-      <c r="AW1" s="11">
+      <c r="AX1" s="11">
         <v>49</v>
       </c>
-      <c r="AX1">
+      <c r="AY1">
         <v>50</v>
       </c>
-      <c r="AY1" s="11">
+      <c r="AZ1" s="11">
         <v>51</v>
       </c>
-      <c r="AZ1">
+      <c r="BA1" s="11">
         <v>52</v>
       </c>
-      <c r="BA1" s="11">
+      <c r="BB1">
         <v>53</v>
       </c>
-      <c r="BB1">
+      <c r="BC1" s="11">
         <v>54</v>
       </c>
-      <c r="BC1" s="11">
+      <c r="BD1" s="11">
         <v>55</v>
       </c>
-      <c r="BD1">
+      <c r="BE1">
         <v>56</v>
       </c>
-      <c r="BE1" s="11">
+      <c r="BF1" s="11">
         <v>57</v>
       </c>
-      <c r="BF1">
+      <c r="BG1" s="11">
         <v>58</v>
       </c>
-      <c r="BG1" s="11">
+      <c r="BH1">
         <v>59</v>
       </c>
-      <c r="BH1">
+      <c r="BI1" s="11">
         <v>60</v>
       </c>
-      <c r="BI1" s="11">
+      <c r="BJ1" s="11">
         <v>61</v>
       </c>
-      <c r="BJ1">
+      <c r="BK1">
         <v>62</v>
       </c>
-      <c r="BK1" s="11">
+      <c r="BL1" s="11">
         <v>63</v>
       </c>
-      <c r="BL1">
+      <c r="BM1" s="11">
         <v>64</v>
       </c>
-      <c r="BM1" s="11">
+    </row>
+    <row r="2" spans="2:65" x14ac:dyDescent="0.15">
+      <c r="B2" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="J2" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="K2" s="15"/>
+    </row>
+    <row r="3" spans="2:65" x14ac:dyDescent="0.15">
+      <c r="B3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="P3" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q3" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="R3" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="S3" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="T3" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="U3" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="V3" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="W3" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="X3" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y3" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z3" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA3" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB3" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC3" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="AD3" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE3" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG3" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH3" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI3" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ3" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK3" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="AL3" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="AM3" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN3" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="AO3" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP3" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="AQ3" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="AR3" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="AS3" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="AT3" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="AU3" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="AV3" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="AW3" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="AX3" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="AY3" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="AZ3" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="BA3" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="BB3" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC3" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="BD3" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="BE3" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="BF3" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="BG3" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="BH3" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="BI3" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="BJ3" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="BK3" s="13" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="2" spans="1:65" x14ac:dyDescent="0.15">
-      <c r="A2" s="12" t="s">
-        <v>183</v>
-      </c>
-      <c r="B2" s="12"/>
-      <c r="AF2" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="AG2" s="12"/>
-    </row>
-    <row r="3" spans="1:65" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>143</v>
-      </c>
-      <c r="E3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" t="s">
-        <v>33</v>
-      </c>
-      <c r="K3" t="s">
-        <v>35</v>
-      </c>
-      <c r="L3" t="s">
-        <v>37</v>
-      </c>
-      <c r="M3" t="s">
-        <v>39</v>
-      </c>
-      <c r="N3" t="s">
-        <v>41</v>
-      </c>
-      <c r="O3" t="s">
-        <v>43</v>
-      </c>
-      <c r="P3" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>47</v>
-      </c>
-      <c r="R3" t="s">
-        <v>49</v>
-      </c>
-      <c r="S3" t="s">
-        <v>51</v>
-      </c>
-      <c r="T3" t="s">
-        <v>53</v>
-      </c>
-      <c r="U3" t="s">
-        <v>55</v>
-      </c>
-      <c r="V3" t="s">
-        <v>57</v>
-      </c>
-      <c r="W3" t="s">
-        <v>59</v>
-      </c>
-      <c r="X3" t="s">
-        <v>61</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>65</v>
-      </c>
-      <c r="AA3" t="s">
+      <c r="BL3" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="BM3" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="AC3" t="s">
-        <v>71</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>73</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>75</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>17</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>19</v>
-      </c>
-      <c r="AI3" t="s">
+    </row>
+    <row r="4" spans="2:65" x14ac:dyDescent="0.15">
+      <c r="B4" s="9">
+        <v>45627</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>154</v>
+      </c>
+      <c r="F4" t="s">
+        <v>174</v>
+      </c>
+      <c r="G4">
+        <v>1105.1500000000001</v>
+      </c>
+      <c r="H4">
         <v>21</v>
       </c>
-      <c r="AJ3" t="s">
-        <v>7</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>135</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>79</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>81</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>77</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>83</v>
-      </c>
-      <c r="AP3" t="s">
-        <v>85</v>
-      </c>
-      <c r="AQ3" t="s">
-        <v>87</v>
-      </c>
-      <c r="AR3" t="s">
-        <v>89</v>
-      </c>
-      <c r="AS3" t="s">
-        <v>91</v>
-      </c>
-      <c r="AT3" t="s">
-        <v>93</v>
-      </c>
-      <c r="AU3" t="s">
-        <v>95</v>
-      </c>
-      <c r="AV3" t="s">
-        <v>97</v>
-      </c>
-      <c r="AW3" t="s">
-        <v>99</v>
-      </c>
-      <c r="AX3" t="s">
-        <v>101</v>
-      </c>
-      <c r="AY3" t="s">
-        <v>103</v>
-      </c>
-      <c r="AZ3" t="s">
-        <v>105</v>
-      </c>
-      <c r="BA3" t="s">
-        <v>107</v>
-      </c>
-      <c r="BB3" t="s">
-        <v>109</v>
-      </c>
-      <c r="BC3" t="s">
-        <v>111</v>
-      </c>
-      <c r="BD3" t="s">
-        <v>113</v>
-      </c>
-      <c r="BE3" t="s">
-        <v>115</v>
-      </c>
-      <c r="BF3" t="s">
-        <v>117</v>
-      </c>
-      <c r="BG3" t="s">
-        <v>119</v>
-      </c>
-      <c r="BH3" t="s">
-        <v>121</v>
-      </c>
-      <c r="BI3" t="s">
-        <v>123</v>
-      </c>
-      <c r="BJ3" t="s">
-        <v>125</v>
-      </c>
-      <c r="BK3" t="s">
-        <v>127</v>
-      </c>
-      <c r="BL3" t="s">
-        <v>129</v>
-      </c>
-      <c r="BM3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="4" spans="1:65" x14ac:dyDescent="0.15">
-      <c r="A4" s="9">
-        <v>45627</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="I4">
+        <f>ROUND(G4*H4/100,2)</f>
+        <v>232.08</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="K4">
+        <v>12</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>160</v>
+      </c>
+      <c r="R4" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="S4" s="10"/>
+      <c r="U4">
+        <f t="shared" ref="U4:U10" si="0">ROUND(G4*T4/100,2)</f>
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>400.33</v>
+      </c>
+      <c r="W4">
+        <v>10</v>
+      </c>
+      <c r="X4">
+        <f>ROUND(V4*W4/100,2)</f>
+        <v>40.03</v>
+      </c>
+      <c r="Z4">
+        <f>ROUND(V4*Y4/100,2)</f>
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>175.8</v>
+      </c>
+      <c r="AB4">
+        <v>4</v>
+      </c>
+      <c r="AC4">
+        <f>ROUND(AA4*AB4/100,2)</f>
+        <v>7.03</v>
+      </c>
+      <c r="AE4">
+        <f>ROUND(AA4*AD4/100,2)</f>
+        <v>0</v>
+      </c>
+      <c r="AF4">
+        <v>750</v>
+      </c>
+      <c r="AG4">
+        <v>0</v>
+      </c>
+      <c r="AH4">
+        <f>ROUND(AF4*AG4/100,2)</f>
+        <v>0</v>
+      </c>
+      <c r="BM4">
+        <f t="shared" ref="BM4:BM10" si="1">G4+I4+U4+V4+X4+Z4+AA4+AC4+AE4+AF4+AH4+AJ4-BL4</f>
+        <v>2710.42</v>
+      </c>
+    </row>
+    <row r="5" spans="2:65" x14ac:dyDescent="0.15">
+      <c r="B5" s="9">
+        <v>45628</v>
+      </c>
+      <c r="C5" t="s">
         <v>3</v>
       </c>
-      <c r="C4">
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F5" t="s">
+        <v>175</v>
+      </c>
+      <c r="G5">
+        <v>400.7</v>
+      </c>
+      <c r="H5">
+        <v>21</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ref="I5:I10" si="2">ROUND(G5*H5/100,2)</f>
+        <v>84.15</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="K5">
+        <v>12</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="M5" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>163</v>
+      </c>
+      <c r="R5" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="S5" s="10"/>
+      <c r="U5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>345.7</v>
+      </c>
+      <c r="W5">
+        <v>10</v>
+      </c>
+      <c r="X5">
+        <f t="shared" ref="X5:X10" si="3">ROUND(V5*W5/100,2)</f>
+        <v>34.57</v>
+      </c>
+      <c r="Z5">
+        <f t="shared" ref="Z5:Z10" si="4">ROUND(V5*Y5/100,2)</f>
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>310.33</v>
+      </c>
+      <c r="AB5">
+        <v>4</v>
+      </c>
+      <c r="AC5">
+        <f t="shared" ref="AC5:AC10" si="5">ROUND(AA5*AB5/100,2)</f>
+        <v>12.41</v>
+      </c>
+      <c r="AE5">
+        <f t="shared" ref="AE5:AE10" si="6">ROUND(AA5*AD5/100,2)</f>
+        <v>0</v>
+      </c>
+      <c r="AH5">
+        <f t="shared" ref="AH5:AH10" si="7">ROUND(AF5*AG5/100,2)</f>
+        <v>0</v>
+      </c>
+      <c r="BM5">
+        <f t="shared" si="1"/>
+        <v>1187.8600000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="2:65" x14ac:dyDescent="0.15">
+      <c r="B6" s="9">
+        <v>45629</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>157</v>
+      </c>
+      <c r="F6" t="s">
+        <v>176</v>
+      </c>
+      <c r="G6">
+        <v>135.77000000000001</v>
+      </c>
+      <c r="H6">
+        <v>21</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>28.51</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="K6">
+        <v>12</v>
+      </c>
+      <c r="L6" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="M6" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>162</v>
+      </c>
+      <c r="R6" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="S6" s="10"/>
+      <c r="U6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>150.12</v>
+      </c>
+      <c r="W6">
+        <v>10</v>
+      </c>
+      <c r="X6">
+        <f t="shared" si="3"/>
+        <v>15.01</v>
+      </c>
+      <c r="Z6">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AC6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AE6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AH6">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="BM6">
+        <f t="shared" si="1"/>
+        <v>329.40999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="2:65" x14ac:dyDescent="0.15">
+      <c r="B7" s="9">
+        <v>45630</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7">
         <v>1</v>
       </c>
-      <c r="D4" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="E4">
-        <v>1105.1500000000001</v>
-      </c>
-      <c r="F4">
+      <c r="E7" t="s">
+        <v>156</v>
+      </c>
+      <c r="F7" t="s">
+        <v>177</v>
+      </c>
+      <c r="G7">
+        <v>2300.14</v>
+      </c>
+      <c r="H7">
         <v>21</v>
       </c>
-      <c r="G4">
-        <f>ROUND(E4*F4/100,2)</f>
-        <v>232.08</v>
-      </c>
-      <c r="I4">
-        <f>ROUND(E4*H4/100,2)</f>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>483.03</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="K7">
+        <v>12</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="N7" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>164</v>
+      </c>
+      <c r="R7" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="S7" s="10"/>
+      <c r="T7">
+        <v>5.2</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="0"/>
+        <v>119.61</v>
+      </c>
+      <c r="V7">
+        <v>170.85</v>
+      </c>
+      <c r="W7">
+        <v>10</v>
+      </c>
+      <c r="X7">
+        <f t="shared" si="3"/>
+        <v>17.09</v>
+      </c>
+      <c r="Y7">
+        <v>1.4</v>
+      </c>
+      <c r="Z7">
+        <f t="shared" si="4"/>
+        <v>2.39</v>
+      </c>
+      <c r="AA7">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="AB7">
+        <v>4</v>
+      </c>
+      <c r="AC7">
+        <f t="shared" si="5"/>
+        <v>1.63</v>
+      </c>
+      <c r="AD7">
+        <v>0.5</v>
+      </c>
+      <c r="AE7">
+        <f t="shared" si="6"/>
+        <v>0.2</v>
+      </c>
+      <c r="AH7">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J4">
-        <v>400.33</v>
-      </c>
-      <c r="K4">
+      <c r="BM7">
+        <f t="shared" si="1"/>
+        <v>3135.7400000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="2:65" x14ac:dyDescent="0.15">
+      <c r="B8" s="9">
+        <v>45630</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>159</v>
+      </c>
+      <c r="F8" t="s">
+        <v>178</v>
+      </c>
+      <c r="G8">
+        <v>1108.0999999999999</v>
+      </c>
+      <c r="H8">
+        <v>21</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>232.7</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="K8">
+        <v>12</v>
+      </c>
+      <c r="L8" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="M8" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="N8" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>165</v>
+      </c>
+      <c r="R8" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="S8" s="10"/>
+      <c r="T8">
+        <v>5.2</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="0"/>
+        <v>57.62</v>
+      </c>
+      <c r="V8">
+        <v>810.2</v>
+      </c>
+      <c r="W8">
         <v>10</v>
       </c>
-      <c r="L4">
-        <f>ROUND(J4*K4/100,2)</f>
-        <v>40.03</v>
-      </c>
-      <c r="N4">
-        <f>ROUND(J4*M4/100,2)</f>
+      <c r="X8">
+        <f t="shared" si="3"/>
+        <v>81.02</v>
+      </c>
+      <c r="Y8">
+        <v>1.4</v>
+      </c>
+      <c r="Z8">
+        <f t="shared" si="4"/>
+        <v>11.34</v>
+      </c>
+      <c r="AA8">
+        <v>91.52</v>
+      </c>
+      <c r="AB8">
+        <v>4</v>
+      </c>
+      <c r="AC8">
+        <f t="shared" si="5"/>
+        <v>3.66</v>
+      </c>
+      <c r="AD8">
+        <v>0.5</v>
+      </c>
+      <c r="AE8">
+        <f t="shared" si="6"/>
+        <v>0.46</v>
+      </c>
+      <c r="AH8">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="O4">
-        <v>175.8</v>
-      </c>
-      <c r="P4">
+      <c r="BM8">
+        <f t="shared" si="1"/>
+        <v>2396.62</v>
+      </c>
+    </row>
+    <row r="9" spans="2:65" x14ac:dyDescent="0.15">
+      <c r="B9" s="9">
+        <v>45631</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9">
         <v>4</v>
       </c>
-      <c r="Q4">
-        <f>ROUND(O4*P4/100,2)</f>
-        <v>7.03</v>
-      </c>
-      <c r="S4">
-        <f>ROUND(O4*R4/100,2)</f>
+      <c r="E9" t="s">
+        <v>158</v>
+      </c>
+      <c r="F9" t="s">
+        <v>179</v>
+      </c>
+      <c r="G9">
+        <v>600.15</v>
+      </c>
+      <c r="H9">
+        <v>21</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>126.03</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="K9">
+        <v>12</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="M9" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="N9" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>161</v>
+      </c>
+      <c r="R9" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="S9" s="10"/>
+      <c r="U9">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T4">
-        <v>750</v>
-      </c>
-      <c r="U4">
-        <v>0</v>
-      </c>
-      <c r="V4">
-        <f>ROUND(T4*U4/100,2)</f>
-        <v>0</v>
-      </c>
-      <c r="AB4">
-        <f>E4+G4+I4+J4+L4+N4+O4+Q4+S4+T4+V4+X4-AA4</f>
-        <v>2710.42</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>154</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>160</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>161</v>
-      </c>
-      <c r="AF4">
-        <v>12</v>
-      </c>
-      <c r="AG4" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="AH4" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="AI4" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>170</v>
-      </c>
-      <c r="AM4" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="AN4" s="10"/>
-    </row>
-    <row r="5" spans="1:65" x14ac:dyDescent="0.15">
-      <c r="A5" s="9">
-        <v>45628</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="E5">
-        <v>400.7</v>
-      </c>
-      <c r="F5">
-        <v>21</v>
-      </c>
-      <c r="G5">
-        <f t="shared" ref="G5:G10" si="0">ROUND(E5*F5/100,2)</f>
-        <v>84.15</v>
-      </c>
-      <c r="I5">
-        <f t="shared" ref="I5:I10" si="1">ROUND(E5*H5/100,2)</f>
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>345.7</v>
-      </c>
-      <c r="K5">
-        <v>10</v>
-      </c>
-      <c r="L5">
-        <f t="shared" ref="L5:L10" si="2">ROUND(J5*K5/100,2)</f>
-        <v>34.57</v>
-      </c>
-      <c r="N5">
-        <f t="shared" ref="N5:N10" si="3">ROUND(J5*M5/100,2)</f>
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <v>310.33</v>
-      </c>
-      <c r="P5">
-        <v>4</v>
-      </c>
-      <c r="Q5">
-        <f t="shared" ref="Q5:Q10" si="4">ROUND(O5*P5/100,2)</f>
-        <v>12.41</v>
-      </c>
-      <c r="S5">
-        <f t="shared" ref="S5:S10" si="5">ROUND(O5*R5/100,2)</f>
-        <v>0</v>
-      </c>
-      <c r="V5">
-        <f t="shared" ref="V5:V10" si="6">ROUND(T5*U5/100,2)</f>
-        <v>0</v>
-      </c>
-      <c r="AB5">
-        <f t="shared" ref="AB5:AB10" si="7">E5+G5+I5+J5+L5+N5+O5+Q5+S5+T5+V5+X5-AA5</f>
-        <v>1187.8600000000001</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>155</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>162</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>163</v>
-      </c>
-      <c r="AF5">
-        <v>12</v>
-      </c>
-      <c r="AG5" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="AH5" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="AI5" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>173</v>
-      </c>
-      <c r="AM5" s="10" t="s">
-        <v>177</v>
-      </c>
-      <c r="AN5" s="10"/>
-    </row>
-    <row r="6" spans="1:65" x14ac:dyDescent="0.15">
-      <c r="A6" s="9">
-        <v>45629</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="E6">
-        <v>135.77000000000001</v>
-      </c>
-      <c r="F6">
-        <v>21</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="0"/>
-        <v>28.51</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>150.12</v>
-      </c>
-      <c r="K6">
-        <v>10</v>
-      </c>
-      <c r="L6">
-        <f t="shared" si="2"/>
-        <v>15.01</v>
-      </c>
-      <c r="N6">
+      <c r="X9">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="Q6">
+      <c r="Z9">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="S6">
+      <c r="AC9">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="V6">
+      <c r="AE9">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AB6">
+      <c r="AH9">
         <f t="shared" si="7"/>
-        <v>329.40999999999997</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>157</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>164</v>
-      </c>
-      <c r="AF6">
+        <v>0</v>
+      </c>
+      <c r="BM9">
+        <f t="shared" si="1"/>
+        <v>726.18</v>
+      </c>
+    </row>
+    <row r="10" spans="2:65" x14ac:dyDescent="0.15">
+      <c r="B10" s="9">
+        <v>45632</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>154</v>
+      </c>
+      <c r="F10" t="s">
+        <v>174</v>
+      </c>
+      <c r="G10">
+        <v>750</v>
+      </c>
+      <c r="H10">
+        <v>21</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>157.5</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="K10">
         <v>12</v>
       </c>
-      <c r="AG6" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="AH6" s="10" t="s">
+      <c r="L10" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="M10" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="AI6" s="10" t="s">
+      <c r="N10" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="AL6" t="s">
-        <v>172</v>
-      </c>
-      <c r="AM6" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="AN6" s="10"/>
-    </row>
-    <row r="7" spans="1:65" x14ac:dyDescent="0.15">
-      <c r="A7" s="9">
-        <v>45630</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="E7">
-        <v>2300.14</v>
-      </c>
-      <c r="F7">
-        <v>21</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="0"/>
-        <v>483.03</v>
-      </c>
-      <c r="H7">
-        <v>5.2</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="1"/>
-        <v>119.61</v>
-      </c>
-      <c r="J7">
-        <v>170.85</v>
-      </c>
-      <c r="K7">
-        <v>10</v>
-      </c>
-      <c r="L7">
-        <f t="shared" si="2"/>
-        <v>17.09</v>
-      </c>
-      <c r="M7">
-        <v>1.4</v>
-      </c>
-      <c r="N7">
+      <c r="Q10" t="s">
+        <v>160</v>
+      </c>
+      <c r="R10" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="S10" s="10"/>
+      <c r="U10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="X10">
         <f t="shared" si="3"/>
-        <v>2.39</v>
-      </c>
-      <c r="O7">
-        <v>40.799999999999997</v>
-      </c>
-      <c r="P7">
-        <v>4</v>
-      </c>
-      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="Z10">
         <f t="shared" si="4"/>
-        <v>1.63</v>
-      </c>
-      <c r="R7">
-        <v>0.5</v>
-      </c>
-      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="AC10">
         <f t="shared" si="5"/>
-        <v>0.2</v>
-      </c>
-      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="AE10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AB7">
+      <c r="AH10">
         <f t="shared" si="7"/>
-        <v>3135.7400000000002</v>
-      </c>
-      <c r="AC7" t="s">
-        <v>156</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>166</v>
-      </c>
-      <c r="AE7" t="s">
-        <v>165</v>
-      </c>
-      <c r="AF7">
-        <v>12</v>
-      </c>
-      <c r="AG7" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="AH7" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="AI7" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="AL7" t="s">
-        <v>174</v>
-      </c>
-      <c r="AM7" s="10" t="s">
-        <v>179</v>
-      </c>
-      <c r="AN7" s="10"/>
-    </row>
-    <row r="8" spans="1:65" x14ac:dyDescent="0.15">
-      <c r="A8" s="9">
-        <v>45630</v>
-      </c>
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="E8">
-        <v>1108.0999999999999</v>
-      </c>
-      <c r="F8">
-        <v>21</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="0"/>
-        <v>232.7</v>
-      </c>
-      <c r="H8">
-        <v>5.2</v>
-      </c>
-      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="BJ10">
+        <v>750</v>
+      </c>
+      <c r="BK10">
+        <v>19</v>
+      </c>
+      <c r="BL10">
+        <f t="shared" ref="BL10" si="8">ROUND(BJ10*BK10/100,2)</f>
+        <v>142.5</v>
+      </c>
+      <c r="BM10">
         <f t="shared" si="1"/>
-        <v>57.62</v>
-      </c>
-      <c r="J8">
-        <v>810.2</v>
-      </c>
-      <c r="K8">
-        <v>10</v>
-      </c>
-      <c r="L8">
-        <f t="shared" si="2"/>
-        <v>81.02</v>
-      </c>
-      <c r="M8">
-        <v>1.4</v>
-      </c>
-      <c r="N8">
-        <f t="shared" si="3"/>
-        <v>11.34</v>
-      </c>
-      <c r="O8">
-        <v>91.52</v>
-      </c>
-      <c r="P8">
-        <v>4</v>
-      </c>
-      <c r="Q8">
-        <f t="shared" si="4"/>
-        <v>3.66</v>
-      </c>
-      <c r="R8">
-        <v>0.5</v>
-      </c>
-      <c r="S8">
-        <f t="shared" si="5"/>
-        <v>0.46</v>
-      </c>
-      <c r="V8">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AB8">
-        <f t="shared" si="7"/>
-        <v>2396.62</v>
-      </c>
-      <c r="AC8" t="s">
-        <v>159</v>
-      </c>
-      <c r="AD8" t="s">
-        <v>167</v>
-      </c>
-      <c r="AE8" t="s">
-        <v>168</v>
-      </c>
-      <c r="AF8">
-        <v>12</v>
-      </c>
-      <c r="AG8" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="AH8" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="AI8" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="AL8" t="s">
-        <v>175</v>
-      </c>
-      <c r="AM8" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="AN8" s="10"/>
-    </row>
-    <row r="9" spans="1:65" x14ac:dyDescent="0.15">
-      <c r="A9" s="9">
-        <v>45631</v>
-      </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9">
-        <v>4</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="E9">
-        <v>600.15</v>
-      </c>
-      <c r="F9">
-        <v>21</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="0"/>
-        <v>126.03</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Q9">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="S9">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="V9">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AB9">
-        <f t="shared" si="7"/>
-        <v>726.18</v>
-      </c>
-      <c r="AC9" t="s">
-        <v>158</v>
-      </c>
-      <c r="AD9" t="s">
-        <v>169</v>
-      </c>
-      <c r="AF9">
-        <v>12</v>
-      </c>
-      <c r="AG9" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="AH9" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="AI9" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="AL9" t="s">
-        <v>171</v>
-      </c>
-      <c r="AM9" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="AN9" s="10"/>
-    </row>
-    <row r="10" spans="1:65" x14ac:dyDescent="0.15">
-      <c r="A10" s="9">
-        <v>45632</v>
-      </c>
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10">
-        <v>5</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="E10">
-        <v>750</v>
-      </c>
-      <c r="F10">
-        <v>21</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="0"/>
-        <v>157.5</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N10">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Q10">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="S10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="V10">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Y10">
-        <v>750</v>
-      </c>
-      <c r="Z10">
-        <v>19</v>
-      </c>
-      <c r="AA10">
-        <f t="shared" ref="AA10" si="8">ROUND(Y10*Z10/100,2)</f>
-        <v>142.5</v>
-      </c>
-      <c r="AB10">
-        <f t="shared" si="7"/>
         <v>765</v>
       </c>
-      <c r="AC10" t="s">
-        <v>154</v>
-      </c>
-      <c r="AD10" t="s">
-        <v>160</v>
-      </c>
-      <c r="AE10" t="s">
-        <v>161</v>
-      </c>
-      <c r="AF10">
-        <v>12</v>
-      </c>
-      <c r="AG10" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="AH10" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="AI10" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="AL10" t="s">
-        <v>170</v>
-      </c>
-      <c r="AM10" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="AN10" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="AF2:AG2"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="J2:K2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Version v1.3.1.0 - Modificados todos los metodos para cambiar el orden de salida y fijar las bases y cuotas 1 a 4 para los tipos habituales (21, 10, 4, y 0) - Realizadas pruebas con los tipos E00, E01 y R00 y son correctas.
</commit_message>
<xml_diff>
--- a/pruebas/emitidasDiagram.xlsx
+++ b/pruebas/emitidasDiagram.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="186">
   <si>
     <t>Columna</t>
   </si>
@@ -543,12 +543,6 @@
     <t>08002</t>
   </si>
   <si>
-    <t>Campos opcionales</t>
-  </si>
-  <si>
-    <t>Campos obligatorios</t>
-  </si>
-  <si>
     <t>APELLIDO APELLIDO, NOMBRE</t>
   </si>
   <si>
@@ -565,6 +559,30 @@
   </si>
   <si>
     <t xml:space="preserve">FRUTOS SECOS MANCHUELA, </t>
+  </si>
+  <si>
+    <t>Obligatorio</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Facturas al 21% fijo</t>
+  </si>
+  <si>
+    <t>Facturas al 10% fijo</t>
+  </si>
+  <si>
+    <t>Facturas al 4% fijo</t>
+  </si>
+  <si>
+    <t>Facturas al 0% (exentas) fijo</t>
+  </si>
+  <si>
+    <t>Tipo libre (obligatorio poner porcentajes)</t>
   </si>
 </sst>
 </file>
@@ -592,7 +610,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -602,18 +620,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -757,13 +763,15 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1045,29 +1053,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:BM10"/>
+  <dimension ref="A1:BM11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="3" max="3" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.75" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.625" customWidth="1"/>
-    <col min="11" max="11" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.75" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="16.875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="12.625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11.625" bestFit="1" customWidth="1"/>
@@ -1116,1035 +1126,1419 @@
     <col min="65" max="65" width="10.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:65" x14ac:dyDescent="0.15">
-      <c r="B1" s="11">
+    <row r="1" spans="1:65" x14ac:dyDescent="0.15">
+      <c r="A1" t="str">
+        <f>IF(COLUMN(A1)&lt;=26, CHAR(64+COLUMN(A1)), CHAR(64+INT((COLUMN(A1)-1)/26))&amp;CHAR(65+MOD(COLUMN(A1)-1,26)))</f>
+        <v>A</v>
+      </c>
+      <c r="B1" t="str">
+        <f t="shared" ref="B1:BM1" si="0">IF(COLUMN(B1)&lt;=26, CHAR(64+COLUMN(B1)), CHAR(64+INT((COLUMN(B1)-1)/26))&amp;CHAR(65+MOD(COLUMN(B1)-1,26)))</f>
+        <v>B</v>
+      </c>
+      <c r="C1" t="str">
+        <f t="shared" si="0"/>
+        <v>C</v>
+      </c>
+      <c r="D1" t="str">
+        <f t="shared" si="0"/>
+        <v>D</v>
+      </c>
+      <c r="E1" t="str">
+        <f t="shared" si="0"/>
+        <v>E</v>
+      </c>
+      <c r="F1" t="str">
+        <f t="shared" si="0"/>
+        <v>F</v>
+      </c>
+      <c r="G1" t="str">
+        <f t="shared" si="0"/>
+        <v>G</v>
+      </c>
+      <c r="H1" t="str">
+        <f t="shared" si="0"/>
+        <v>H</v>
+      </c>
+      <c r="I1" t="str">
+        <f t="shared" si="0"/>
+        <v>I</v>
+      </c>
+      <c r="J1" t="str">
+        <f t="shared" si="0"/>
+        <v>J</v>
+      </c>
+      <c r="K1" t="str">
+        <f t="shared" si="0"/>
+        <v>K</v>
+      </c>
+      <c r="L1" t="str">
+        <f t="shared" si="0"/>
+        <v>L</v>
+      </c>
+      <c r="M1" t="str">
+        <f t="shared" si="0"/>
+        <v>M</v>
+      </c>
+      <c r="N1" t="str">
+        <f t="shared" si="0"/>
+        <v>N</v>
+      </c>
+      <c r="O1" t="str">
+        <f t="shared" si="0"/>
+        <v>O</v>
+      </c>
+      <c r="P1" t="str">
+        <f t="shared" si="0"/>
+        <v>P</v>
+      </c>
+      <c r="Q1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q</v>
+      </c>
+      <c r="R1" t="str">
+        <f t="shared" si="0"/>
+        <v>R</v>
+      </c>
+      <c r="S1" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+      <c r="T1" t="str">
+        <f t="shared" si="0"/>
+        <v>T</v>
+      </c>
+      <c r="U1" t="str">
+        <f t="shared" si="0"/>
+        <v>U</v>
+      </c>
+      <c r="V1" t="str">
+        <f t="shared" si="0"/>
+        <v>V</v>
+      </c>
+      <c r="W1" t="str">
+        <f t="shared" si="0"/>
+        <v>W</v>
+      </c>
+      <c r="X1" t="str">
+        <f t="shared" si="0"/>
+        <v>X</v>
+      </c>
+      <c r="Y1" t="str">
+        <f t="shared" si="0"/>
+        <v>Y</v>
+      </c>
+      <c r="Z1" t="str">
+        <f t="shared" si="0"/>
+        <v>Z</v>
+      </c>
+      <c r="AA1" t="str">
+        <f t="shared" si="0"/>
+        <v>AA</v>
+      </c>
+      <c r="AB1" t="str">
+        <f t="shared" si="0"/>
+        <v>AB</v>
+      </c>
+      <c r="AC1" t="str">
+        <f t="shared" si="0"/>
+        <v>AC</v>
+      </c>
+      <c r="AD1" t="str">
+        <f t="shared" si="0"/>
+        <v>AD</v>
+      </c>
+      <c r="AE1" t="str">
+        <f t="shared" si="0"/>
+        <v>AE</v>
+      </c>
+      <c r="AF1" t="str">
+        <f t="shared" si="0"/>
+        <v>AF</v>
+      </c>
+      <c r="AG1" t="str">
+        <f t="shared" si="0"/>
+        <v>AG</v>
+      </c>
+      <c r="AH1" t="str">
+        <f t="shared" si="0"/>
+        <v>AH</v>
+      </c>
+      <c r="AI1" t="str">
+        <f t="shared" si="0"/>
+        <v>AI</v>
+      </c>
+      <c r="AJ1" t="str">
+        <f t="shared" si="0"/>
+        <v>AJ</v>
+      </c>
+      <c r="AK1" t="str">
+        <f t="shared" si="0"/>
+        <v>AK</v>
+      </c>
+      <c r="AL1" t="str">
+        <f t="shared" si="0"/>
+        <v>AL</v>
+      </c>
+      <c r="AM1" t="str">
+        <f t="shared" si="0"/>
+        <v>AM</v>
+      </c>
+      <c r="AN1" t="str">
+        <f t="shared" si="0"/>
+        <v>AN</v>
+      </c>
+      <c r="AO1" t="str">
+        <f t="shared" si="0"/>
+        <v>AO</v>
+      </c>
+      <c r="AP1" t="str">
+        <f t="shared" si="0"/>
+        <v>AP</v>
+      </c>
+      <c r="AQ1" t="str">
+        <f t="shared" si="0"/>
+        <v>AQ</v>
+      </c>
+      <c r="AR1" t="str">
+        <f t="shared" si="0"/>
+        <v>AR</v>
+      </c>
+      <c r="AS1" t="str">
+        <f t="shared" si="0"/>
+        <v>AS</v>
+      </c>
+      <c r="AT1" t="str">
+        <f t="shared" si="0"/>
+        <v>AT</v>
+      </c>
+      <c r="AU1" t="str">
+        <f t="shared" si="0"/>
+        <v>AU</v>
+      </c>
+      <c r="AV1" t="str">
+        <f t="shared" si="0"/>
+        <v>AV</v>
+      </c>
+      <c r="AW1" t="str">
+        <f t="shared" si="0"/>
+        <v>AW</v>
+      </c>
+      <c r="AX1" t="str">
+        <f t="shared" si="0"/>
+        <v>AX</v>
+      </c>
+      <c r="AY1" t="str">
+        <f t="shared" si="0"/>
+        <v>AY</v>
+      </c>
+      <c r="AZ1" t="str">
+        <f t="shared" si="0"/>
+        <v>AZ</v>
+      </c>
+      <c r="BA1" t="str">
+        <f t="shared" si="0"/>
+        <v>BA</v>
+      </c>
+      <c r="BB1" t="str">
+        <f t="shared" si="0"/>
+        <v>BB</v>
+      </c>
+      <c r="BC1" t="str">
+        <f t="shared" si="0"/>
+        <v>BC</v>
+      </c>
+      <c r="BD1" t="str">
+        <f t="shared" si="0"/>
+        <v>BD</v>
+      </c>
+      <c r="BE1" t="str">
+        <f t="shared" si="0"/>
+        <v>BE</v>
+      </c>
+      <c r="BF1" t="str">
+        <f t="shared" si="0"/>
+        <v>BF</v>
+      </c>
+      <c r="BG1" t="str">
+        <f t="shared" si="0"/>
+        <v>BG</v>
+      </c>
+      <c r="BH1" t="str">
+        <f t="shared" si="0"/>
+        <v>BH</v>
+      </c>
+      <c r="BI1" t="str">
+        <f t="shared" si="0"/>
+        <v>BI</v>
+      </c>
+      <c r="BJ1" t="str">
+        <f t="shared" si="0"/>
+        <v>BJ</v>
+      </c>
+      <c r="BK1" t="str">
+        <f t="shared" si="0"/>
+        <v>BK</v>
+      </c>
+      <c r="BL1" t="str">
+        <f t="shared" si="0"/>
+        <v>BL</v>
+      </c>
+      <c r="BM1" t="str">
+        <f t="shared" si="0"/>
+        <v>BM</v>
+      </c>
+    </row>
+    <row r="2" spans="1:65" x14ac:dyDescent="0.15">
+      <c r="B2" s="11">
         <v>1</v>
       </c>
-      <c r="C1">
+      <c r="C2" s="11">
         <v>2</v>
       </c>
-      <c r="D1" s="11">
+      <c r="D2" s="11">
         <v>3</v>
       </c>
-      <c r="E1" s="11">
+      <c r="E2" s="11">
         <v>4</v>
       </c>
-      <c r="F1">
+      <c r="F2" s="11">
         <v>5</v>
       </c>
-      <c r="G1" s="11">
+      <c r="G2" s="11">
         <v>6</v>
       </c>
-      <c r="H1" s="11">
+      <c r="H2" s="11">
         <v>7</v>
       </c>
-      <c r="I1">
+      <c r="I2" s="11">
         <v>8</v>
       </c>
-      <c r="J1" s="11">
+      <c r="J2" s="11">
         <v>9</v>
       </c>
-      <c r="K1" s="11">
+      <c r="K2" s="11">
         <v>10</v>
       </c>
-      <c r="L1">
+      <c r="L2" s="11">
         <v>11</v>
       </c>
-      <c r="M1" s="11">
+      <c r="M2" s="11">
         <v>12</v>
       </c>
-      <c r="N1" s="11">
+      <c r="N2" s="11">
         <v>13</v>
       </c>
-      <c r="O1">
+      <c r="O2" s="11">
         <v>14</v>
       </c>
-      <c r="P1" s="11">
+      <c r="P2" s="11">
         <v>15</v>
       </c>
-      <c r="Q1" s="11">
+      <c r="Q2" s="11">
         <v>16</v>
       </c>
-      <c r="R1">
+      <c r="R2" s="11">
         <v>17</v>
       </c>
-      <c r="S1" s="11">
+      <c r="S2" s="11">
         <v>18</v>
       </c>
-      <c r="T1" s="11">
+      <c r="T2" s="11">
         <v>19</v>
       </c>
-      <c r="U1">
+      <c r="U2" s="11">
         <v>20</v>
       </c>
-      <c r="V1" s="11">
+      <c r="V2" s="11">
         <v>21</v>
       </c>
-      <c r="W1" s="11">
+      <c r="W2" s="11">
         <v>22</v>
       </c>
-      <c r="X1">
+      <c r="X2" s="11">
         <v>23</v>
       </c>
-      <c r="Y1" s="11">
+      <c r="Y2" s="11">
         <v>24</v>
       </c>
-      <c r="Z1" s="11">
+      <c r="Z2" s="11">
         <v>25</v>
       </c>
-      <c r="AA1">
+      <c r="AA2" s="11">
         <v>26</v>
       </c>
-      <c r="AB1" s="11">
+      <c r="AB2" s="11">
         <v>27</v>
       </c>
-      <c r="AC1" s="11">
+      <c r="AC2" s="11">
         <v>28</v>
       </c>
-      <c r="AD1">
+      <c r="AD2" s="11">
         <v>29</v>
       </c>
-      <c r="AE1" s="11">
+      <c r="AE2" s="11">
         <v>30</v>
       </c>
-      <c r="AF1" s="11">
+      <c r="AF2" s="11">
         <v>31</v>
       </c>
-      <c r="AG1">
+      <c r="AG2" s="11">
         <v>32</v>
       </c>
-      <c r="AH1" s="11">
+      <c r="AH2" s="11">
         <v>33</v>
       </c>
-      <c r="AI1" s="11">
+      <c r="AI2" s="11">
         <v>34</v>
       </c>
-      <c r="AJ1">
+      <c r="AJ2" s="11">
         <v>35</v>
       </c>
-      <c r="AK1" s="11">
+      <c r="AK2" s="11">
         <v>36</v>
       </c>
-      <c r="AL1" s="11">
+      <c r="AL2" s="11">
         <v>37</v>
       </c>
-      <c r="AM1">
+      <c r="AM2" s="11">
         <v>38</v>
       </c>
-      <c r="AN1" s="11">
+      <c r="AN2" s="11">
         <v>39</v>
       </c>
-      <c r="AO1" s="11">
+      <c r="AO2" s="11">
         <v>40</v>
       </c>
-      <c r="AP1">
+      <c r="AP2" s="11">
         <v>41</v>
       </c>
-      <c r="AQ1" s="11">
+      <c r="AQ2" s="11">
         <v>42</v>
       </c>
-      <c r="AR1" s="11">
+      <c r="AR2" s="11">
         <v>43</v>
       </c>
-      <c r="AS1">
+      <c r="AS2" s="11">
         <v>44</v>
       </c>
-      <c r="AT1" s="11">
+      <c r="AT2" s="11">
         <v>45</v>
       </c>
-      <c r="AU1" s="11">
+      <c r="AU2" s="11">
         <v>46</v>
       </c>
-      <c r="AV1">
+      <c r="AV2" s="11">
         <v>47</v>
       </c>
-      <c r="AW1" s="11">
+      <c r="AW2" s="11">
         <v>48</v>
       </c>
-      <c r="AX1" s="11">
+      <c r="AX2" s="11">
         <v>49</v>
       </c>
-      <c r="AY1">
+      <c r="AY2" s="11">
         <v>50</v>
       </c>
-      <c r="AZ1" s="11">
+      <c r="AZ2" s="11">
         <v>51</v>
       </c>
-      <c r="BA1" s="11">
+      <c r="BA2" s="11">
         <v>52</v>
       </c>
-      <c r="BB1">
+      <c r="BB2" s="11">
         <v>53</v>
       </c>
-      <c r="BC1" s="11">
+      <c r="BC2" s="11">
         <v>54</v>
       </c>
-      <c r="BD1" s="11">
+      <c r="BD2" s="11">
         <v>55</v>
       </c>
-      <c r="BE1">
+      <c r="BE2" s="11">
         <v>56</v>
       </c>
-      <c r="BF1" s="11">
+      <c r="BF2" s="11">
         <v>57</v>
       </c>
-      <c r="BG1" s="11">
+      <c r="BG2" s="11">
         <v>58</v>
       </c>
-      <c r="BH1">
+      <c r="BH2" s="11">
         <v>59</v>
       </c>
-      <c r="BI1" s="11">
+      <c r="BI2" s="11">
         <v>60</v>
       </c>
-      <c r="BJ1" s="11">
+      <c r="BJ2" s="11">
         <v>61</v>
       </c>
-      <c r="BK1">
+      <c r="BK2" s="11">
         <v>62</v>
       </c>
-      <c r="BL1" s="11">
+      <c r="BL2" s="11">
         <v>63</v>
       </c>
-      <c r="BM1" s="11">
+      <c r="BM2" s="11">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="2:65" x14ac:dyDescent="0.15">
-      <c r="B2" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="C2" s="14"/>
-      <c r="J2" s="15" t="s">
+    <row r="3" spans="1:65" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="P3" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="Q3" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="R3" s="14"/>
+      <c r="S3" s="14"/>
+      <c r="T3" s="14"/>
+      <c r="U3" s="14"/>
+      <c r="V3" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="W3" s="14"/>
+      <c r="X3" s="14"/>
+      <c r="Y3" s="14"/>
+      <c r="Z3" s="14"/>
+      <c r="AA3" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="AB3" s="14"/>
+      <c r="AC3" s="14"/>
+      <c r="AD3" s="14"/>
+      <c r="AE3" s="14"/>
+      <c r="AF3" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="AG3" s="14"/>
+      <c r="AH3" s="14"/>
+      <c r="AI3" s="14"/>
+      <c r="AJ3" s="14"/>
+      <c r="AK3" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="AL3" s="15"/>
+      <c r="AM3" s="15"/>
+      <c r="AN3" s="15"/>
+      <c r="AO3" s="15"/>
+      <c r="AP3" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="AQ3" s="15"/>
+      <c r="AR3" s="15"/>
+      <c r="AS3" s="15"/>
+      <c r="AT3" s="15"/>
+      <c r="AU3" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="AV3" s="15"/>
+      <c r="AW3" s="15"/>
+      <c r="AX3" s="15"/>
+      <c r="AY3" s="15"/>
+      <c r="AZ3" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="BA3" s="15"/>
+      <c r="BB3" s="15"/>
+      <c r="BC3" s="15"/>
+      <c r="BD3" s="15"/>
+      <c r="BE3" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="BF3" s="15"/>
+      <c r="BG3" s="15"/>
+      <c r="BH3" s="15"/>
+      <c r="BI3" s="15"/>
+      <c r="BJ3" t="s">
+        <v>180</v>
+      </c>
+      <c r="BK3" t="s">
+        <v>180</v>
+      </c>
+      <c r="BL3" t="s">
+        <v>180</v>
+      </c>
+      <c r="BM3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:65" x14ac:dyDescent="0.15">
+      <c r="B4" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="P4" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q4" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="R4" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="S4" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="T4" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="U4" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="V4" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="W4" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="X4" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y4" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z4" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA4" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB4" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC4" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="AD4" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE4" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF4" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG4" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH4" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI4" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ4" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK4" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="AL4" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="AM4" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN4" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="AO4" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP4" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="AQ4" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="AR4" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="AS4" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="AT4" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="AU4" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="AV4" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="AW4" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="AX4" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="AY4" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="AZ4" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="BA4" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="BB4" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC4" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="BD4" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="BE4" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="BF4" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="BG4" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="BH4" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="BI4" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="BJ4" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="BK4" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="BL4" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="BM4" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:65" x14ac:dyDescent="0.15">
+      <c r="B5" s="9">
+        <v>45627</v>
+      </c>
+      <c r="D5">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="H5" t="s">
+        <v>154</v>
+      </c>
+      <c r="I5" t="s">
         <v>172</v>
       </c>
-      <c r="K2" s="15"/>
-    </row>
-    <row r="3" spans="2:65" x14ac:dyDescent="0.15">
-      <c r="B3" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="K3" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="L3" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="M3" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="N3" s="13" t="s">
+      <c r="J5" t="s">
+        <v>160</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="O5" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q5">
+        <v>1105.1500000000001</v>
+      </c>
+      <c r="R5">
         <v>21</v>
       </c>
-      <c r="O3" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="P3" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="Q3" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="R3" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="S3" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="T3" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="U3" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="V3" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="W3" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="X3" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y3" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z3" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA3" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB3" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC3" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="AD3" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="AE3" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="AF3" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG3" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="AH3" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="AI3" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="AJ3" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="AK3" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="AL3" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="AM3" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="AN3" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="AO3" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="AP3" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="AQ3" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="AR3" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="AS3" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="AT3" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="AU3" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="AV3" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="AW3" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="AX3" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="AY3" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="AZ3" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="BA3" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="BB3" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="BC3" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="BD3" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="BE3" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="BF3" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="BG3" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="BH3" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="BI3" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="BJ3" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="BK3" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="BL3" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="BM3" s="13" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="2:65" x14ac:dyDescent="0.15">
-      <c r="B4" s="9">
-        <v>45627</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>154</v>
-      </c>
-      <c r="F4" t="s">
-        <v>174</v>
-      </c>
-      <c r="G4">
-        <v>1105.1500000000001</v>
-      </c>
-      <c r="H4">
-        <v>21</v>
-      </c>
-      <c r="I4">
-        <f>ROUND(G4*H4/100,2)</f>
+      <c r="S5">
+        <f>ROUND(Q5*R5/100,2)</f>
         <v>232.08</v>
       </c>
-      <c r="J4" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="K4">
-        <v>12</v>
-      </c>
-      <c r="L4" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="M4" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="N4" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>160</v>
-      </c>
-      <c r="R4" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="S4" s="10"/>
-      <c r="U4">
-        <f t="shared" ref="U4:U10" si="0">ROUND(G4*T4/100,2)</f>
+      <c r="U5">
+        <f>ROUND(Q5*T5/100,2)</f>
         <v>0</v>
       </c>
-      <c r="V4">
+      <c r="V5">
         <v>400.33</v>
-      </c>
-      <c r="W4">
-        <v>10</v>
-      </c>
-      <c r="X4">
-        <f>ROUND(V4*W4/100,2)</f>
-        <v>40.03</v>
-      </c>
-      <c r="Z4">
-        <f>ROUND(V4*Y4/100,2)</f>
-        <v>0</v>
-      </c>
-      <c r="AA4">
-        <v>175.8</v>
-      </c>
-      <c r="AB4">
-        <v>4</v>
-      </c>
-      <c r="AC4">
-        <f>ROUND(AA4*AB4/100,2)</f>
-        <v>7.03</v>
-      </c>
-      <c r="AE4">
-        <f>ROUND(AA4*AD4/100,2)</f>
-        <v>0</v>
-      </c>
-      <c r="AF4">
-        <v>750</v>
-      </c>
-      <c r="AG4">
-        <v>0</v>
-      </c>
-      <c r="AH4">
-        <f>ROUND(AF4*AG4/100,2)</f>
-        <v>0</v>
-      </c>
-      <c r="BM4">
-        <f t="shared" ref="BM4:BM10" si="1">G4+I4+U4+V4+X4+Z4+AA4+AC4+AE4+AF4+AH4+AJ4-BL4</f>
-        <v>2710.42</v>
-      </c>
-    </row>
-    <row r="5" spans="2:65" x14ac:dyDescent="0.15">
-      <c r="B5" s="9">
-        <v>45628</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5" t="s">
-        <v>155</v>
-      </c>
-      <c r="F5" t="s">
-        <v>175</v>
-      </c>
-      <c r="G5">
-        <v>400.7</v>
-      </c>
-      <c r="H5">
-        <v>21</v>
-      </c>
-      <c r="I5">
-        <f t="shared" ref="I5:I10" si="2">ROUND(G5*H5/100,2)</f>
-        <v>84.15</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="K5">
-        <v>12</v>
-      </c>
-      <c r="L5" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="M5" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="N5" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>163</v>
-      </c>
-      <c r="R5" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="S5" s="10"/>
-      <c r="U5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="V5">
-        <v>345.7</v>
       </c>
       <c r="W5">
         <v>10</v>
       </c>
       <c r="X5">
-        <f t="shared" ref="X5:X10" si="3">ROUND(V5*W5/100,2)</f>
-        <v>34.57</v>
+        <f>ROUND(V5*W5/100,2)</f>
+        <v>40.03</v>
       </c>
       <c r="Z5">
-        <f t="shared" ref="Z5:Z10" si="4">ROUND(V5*Y5/100,2)</f>
+        <f>ROUND(V5*Y5/100,2)</f>
         <v>0</v>
       </c>
       <c r="AA5">
-        <v>310.33</v>
+        <v>175.8</v>
       </c>
       <c r="AB5">
         <v>4</v>
       </c>
       <c r="AC5">
-        <f t="shared" ref="AC5:AC10" si="5">ROUND(AA5*AB5/100,2)</f>
-        <v>12.41</v>
+        <f>ROUND(AA5*AB5/100,2)</f>
+        <v>7.03</v>
       </c>
       <c r="AE5">
-        <f t="shared" ref="AE5:AE10" si="6">ROUND(AA5*AD5/100,2)</f>
+        <f>ROUND(AA5*AD5/100,2)</f>
         <v>0</v>
       </c>
+      <c r="AF5">
+        <v>750</v>
+      </c>
+      <c r="AG5">
+        <v>0</v>
+      </c>
       <c r="AH5">
-        <f t="shared" ref="AH5:AH10" si="7">ROUND(AF5*AG5/100,2)</f>
+        <f>ROUND(AF5*AG5/100,2)</f>
         <v>0</v>
       </c>
       <c r="BM5">
-        <f t="shared" si="1"/>
-        <v>1187.8600000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="2:65" x14ac:dyDescent="0.15">
+        <f>Q5+S5+U5+V5+X5+Z5+AA5+AC5+AE5+AF5+AH5+AJ5-BL5</f>
+        <v>2710.42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:65" x14ac:dyDescent="0.15">
       <c r="B6" s="9">
-        <v>45629</v>
-      </c>
-      <c r="C6" t="s">
+        <v>45628</v>
+      </c>
+      <c r="D6">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
         <v>3</v>
       </c>
-      <c r="D6">
-        <v>3</v>
-      </c>
-      <c r="E6" t="s">
-        <v>157</v>
-      </c>
-      <c r="F6" t="s">
-        <v>176</v>
-      </c>
-      <c r="G6">
-        <v>135.77000000000001</v>
-      </c>
-      <c r="H6">
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="H6" t="s">
+        <v>155</v>
+      </c>
+      <c r="I6" t="s">
+        <v>173</v>
+      </c>
+      <c r="J6" t="s">
+        <v>163</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="O6" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q6">
+        <v>400.7</v>
+      </c>
+      <c r="R6">
         <v>21</v>
       </c>
-      <c r="I6">
-        <f t="shared" si="2"/>
-        <v>28.51</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="K6">
-        <v>12</v>
-      </c>
-      <c r="L6" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="M6" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="N6" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>162</v>
-      </c>
-      <c r="R6" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="S6" s="10"/>
+      <c r="S6">
+        <f t="shared" ref="S6:S11" si="1">ROUND(Q6*R6/100,2)</f>
+        <v>84.15</v>
+      </c>
       <c r="U6">
-        <f t="shared" si="0"/>
+        <f>ROUND(Q6*T6/100,2)</f>
         <v>0</v>
       </c>
       <c r="V6">
-        <v>150.12</v>
+        <v>345.7</v>
       </c>
       <c r="W6">
         <v>10</v>
       </c>
       <c r="X6">
+        <f t="shared" ref="X6:X11" si="2">ROUND(V6*W6/100,2)</f>
+        <v>34.57</v>
+      </c>
+      <c r="Z6">
+        <f t="shared" ref="Z6:Z11" si="3">ROUND(V6*Y6/100,2)</f>
+        <v>0</v>
+      </c>
+      <c r="AA6">
+        <v>310.33</v>
+      </c>
+      <c r="AB6">
+        <v>4</v>
+      </c>
+      <c r="AC6">
+        <f t="shared" ref="AC6:AC11" si="4">ROUND(AA6*AB6/100,2)</f>
+        <v>12.41</v>
+      </c>
+      <c r="AE6">
+        <f t="shared" ref="AE6:AE11" si="5">ROUND(AA6*AD6/100,2)</f>
+        <v>0</v>
+      </c>
+      <c r="AH6">
+        <f t="shared" ref="AH6:AH11" si="6">ROUND(AF6*AG6/100,2)</f>
+        <v>0</v>
+      </c>
+      <c r="BM6">
+        <f>Q6+S6+U6+V6+X6+Z6+AA6+AC6+AE6+AF6+AH6+AJ6-BL6</f>
+        <v>1187.8600000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:65" x14ac:dyDescent="0.15">
+      <c r="B7" s="9">
+        <v>45629</v>
+      </c>
+      <c r="D7">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="H7" t="s">
+        <v>157</v>
+      </c>
+      <c r="I7" t="s">
+        <v>174</v>
+      </c>
+      <c r="J7" t="s">
+        <v>162</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="N7" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="O7" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q7">
+        <v>135.77000000000001</v>
+      </c>
+      <c r="R7">
+        <v>21</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="1"/>
+        <v>28.51</v>
+      </c>
+      <c r="U7">
+        <f>ROUND(Q7*T7/100,2)</f>
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>150.12</v>
+      </c>
+      <c r="W7">
+        <v>10</v>
+      </c>
+      <c r="X7">
+        <f t="shared" si="2"/>
+        <v>15.01</v>
+      </c>
+      <c r="Z7">
         <f t="shared" si="3"/>
-        <v>15.01</v>
-      </c>
-      <c r="Z6">
+        <v>0</v>
+      </c>
+      <c r="AC7">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AC6">
+      <c r="AE7">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AE6">
+      <c r="AH7">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AH6">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="BM6">
-        <f t="shared" si="1"/>
+      <c r="BM7">
+        <f>Q7+S7+U7+V7+X7+Z7+AA7+AC7+AE7+AF7+AH7+AJ7-BL7</f>
         <v>329.40999999999997</v>
       </c>
     </row>
-    <row r="7" spans="2:65" x14ac:dyDescent="0.15">
-      <c r="B7" s="9">
-        <v>45630</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>156</v>
-      </c>
-      <c r="F7" t="s">
-        <v>177</v>
-      </c>
-      <c r="G7">
-        <v>2300.14</v>
-      </c>
-      <c r="H7">
-        <v>21</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="2"/>
-        <v>483.03</v>
-      </c>
-      <c r="J7" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="K7">
-        <v>12</v>
-      </c>
-      <c r="L7" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="M7" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="N7" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>164</v>
-      </c>
-      <c r="R7" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="S7" s="10"/>
-      <c r="T7">
-        <v>5.2</v>
-      </c>
-      <c r="U7">
-        <f t="shared" si="0"/>
-        <v>119.61</v>
-      </c>
-      <c r="V7">
-        <v>170.85</v>
-      </c>
-      <c r="W7">
-        <v>10</v>
-      </c>
-      <c r="X7">
-        <f t="shared" si="3"/>
-        <v>17.09</v>
-      </c>
-      <c r="Y7">
-        <v>1.4</v>
-      </c>
-      <c r="Z7">
-        <f t="shared" si="4"/>
-        <v>2.39</v>
-      </c>
-      <c r="AA7">
-        <v>40.799999999999997</v>
-      </c>
-      <c r="AB7">
-        <v>4</v>
-      </c>
-      <c r="AC7">
-        <f t="shared" si="5"/>
-        <v>1.63</v>
-      </c>
-      <c r="AD7">
-        <v>0.5</v>
-      </c>
-      <c r="AE7">
-        <f t="shared" si="6"/>
-        <v>0.2</v>
-      </c>
-      <c r="AH7">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="BM7">
-        <f t="shared" si="1"/>
-        <v>3135.7400000000002</v>
-      </c>
-    </row>
-    <row r="8" spans="2:65" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:65" x14ac:dyDescent="0.15">
       <c r="B8" s="9">
         <v>45630</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
         <v>4</v>
       </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8" t="s">
-        <v>159</v>
-      </c>
-      <c r="F8" t="s">
-        <v>178</v>
-      </c>
-      <c r="G8">
-        <v>1108.0999999999999</v>
-      </c>
-      <c r="H8">
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="H8" t="s">
+        <v>156</v>
+      </c>
+      <c r="I8" t="s">
+        <v>175</v>
+      </c>
+      <c r="J8" t="s">
+        <v>164</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="N8" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="O8" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q8">
+        <v>2300.14</v>
+      </c>
+      <c r="R8">
         <v>21</v>
       </c>
-      <c r="I8">
-        <f t="shared" si="2"/>
-        <v>232.7</v>
-      </c>
-      <c r="J8" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="K8">
-        <v>12</v>
-      </c>
-      <c r="L8" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="M8" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="N8" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>165</v>
-      </c>
-      <c r="R8" s="10" t="s">
-        <v>170</v>
-      </c>
-      <c r="S8" s="10"/>
+      <c r="S8">
+        <f t="shared" si="1"/>
+        <v>483.03</v>
+      </c>
       <c r="T8">
         <v>5.2</v>
       </c>
       <c r="U8">
-        <f t="shared" si="0"/>
-        <v>57.62</v>
+        <f>ROUND(Q8*T8/100,2)</f>
+        <v>119.61</v>
       </c>
       <c r="V8">
-        <v>810.2</v>
+        <v>170.85</v>
       </c>
       <c r="W8">
         <v>10</v>
       </c>
       <c r="X8">
-        <f t="shared" si="3"/>
-        <v>81.02</v>
+        <f t="shared" si="2"/>
+        <v>17.09</v>
       </c>
       <c r="Y8">
         <v>1.4</v>
       </c>
       <c r="Z8">
-        <f t="shared" si="4"/>
-        <v>11.34</v>
+        <f t="shared" si="3"/>
+        <v>2.39</v>
       </c>
       <c r="AA8">
-        <v>91.52</v>
+        <v>40.799999999999997</v>
       </c>
       <c r="AB8">
         <v>4</v>
       </c>
       <c r="AC8">
-        <f t="shared" si="5"/>
-        <v>3.66</v>
+        <f t="shared" si="4"/>
+        <v>1.63</v>
       </c>
       <c r="AD8">
         <v>0.5</v>
       </c>
       <c r="AE8">
+        <f t="shared" si="5"/>
+        <v>0.2</v>
+      </c>
+      <c r="AH8">
         <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="BM8">
+        <f>Q8+S8+U8+V8+X8+Z8+AA8+AC8+AE8+AF8+AH8+AJ8-BL8</f>
+        <v>3135.7400000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:65" x14ac:dyDescent="0.15">
+      <c r="B9" s="9">
+        <v>45630</v>
+      </c>
+      <c r="D9">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="H9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I9" t="s">
+        <v>176</v>
+      </c>
+      <c r="J9" t="s">
+        <v>165</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="N9" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="O9" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q9">
+        <v>1108.0999999999999</v>
+      </c>
+      <c r="R9">
+        <v>21</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="1"/>
+        <v>232.7</v>
+      </c>
+      <c r="T9">
+        <v>5.2</v>
+      </c>
+      <c r="U9">
+        <f>ROUND(Q9*T9/100,2)</f>
+        <v>57.62</v>
+      </c>
+      <c r="V9">
+        <v>810.2</v>
+      </c>
+      <c r="W9">
+        <v>10</v>
+      </c>
+      <c r="X9">
+        <f t="shared" si="2"/>
+        <v>81.02</v>
+      </c>
+      <c r="Y9">
+        <v>1.4</v>
+      </c>
+      <c r="Z9">
+        <f t="shared" si="3"/>
+        <v>11.34</v>
+      </c>
+      <c r="AA9">
+        <v>91.52</v>
+      </c>
+      <c r="AB9">
+        <v>4</v>
+      </c>
+      <c r="AC9">
+        <f t="shared" si="4"/>
+        <v>3.66</v>
+      </c>
+      <c r="AD9">
+        <v>0.5</v>
+      </c>
+      <c r="AE9">
+        <f t="shared" si="5"/>
         <v>0.46</v>
       </c>
-      <c r="AH8">
-        <f t="shared" si="7"/>
+      <c r="AH9">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="BM8">
+      <c r="BM9">
+        <f>Q9+S9+U9+V9+X9+Z9+AA9+AC9+AE9+AF9+AH9+AJ9-BL9</f>
+        <v>2396.62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:65" x14ac:dyDescent="0.15">
+      <c r="B10" s="9">
+        <v>45631</v>
+      </c>
+      <c r="D10">
+        <v>12</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <v>4</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="H10" t="s">
+        <v>158</v>
+      </c>
+      <c r="I10" t="s">
+        <v>177</v>
+      </c>
+      <c r="J10" t="s">
+        <v>161</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="N10" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="O10" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q10">
+        <v>600.15</v>
+      </c>
+      <c r="R10">
+        <v>21</v>
+      </c>
+      <c r="S10">
         <f t="shared" si="1"/>
-        <v>2396.62</v>
-      </c>
-    </row>
-    <row r="9" spans="2:65" x14ac:dyDescent="0.15">
-      <c r="B9" s="9">
-        <v>45631</v>
-      </c>
-      <c r="C9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9">
-        <v>4</v>
-      </c>
-      <c r="E9" t="s">
-        <v>158</v>
-      </c>
-      <c r="F9" t="s">
-        <v>179</v>
-      </c>
-      <c r="G9">
-        <v>600.15</v>
-      </c>
-      <c r="H9">
-        <v>21</v>
-      </c>
-      <c r="I9">
+        <v>126.03</v>
+      </c>
+      <c r="U10">
+        <f>ROUND(Q10*T10/100,2)</f>
+        <v>0</v>
+      </c>
+      <c r="X10">
         <f t="shared" si="2"/>
-        <v>126.03</v>
-      </c>
-      <c r="J9" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="K9">
-        <v>12</v>
-      </c>
-      <c r="L9" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="M9" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="N9" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>161</v>
-      </c>
-      <c r="R9" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="S9" s="10"/>
-      <c r="U9">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="X9">
+      <c r="Z10">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="Z9">
+      <c r="AC10">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AC9">
+      <c r="AE10">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AE9">
+      <c r="AH10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AH9">
-        <f t="shared" si="7"/>
+      <c r="BM10">
+        <f>Q10+S10+U10+V10+X10+Z10+AA10+AC10+AE10+AF10+AH10+AJ10-BL10</f>
+        <v>726.18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:65" x14ac:dyDescent="0.15">
+      <c r="B11" s="9">
+        <v>45632</v>
+      </c>
+      <c r="D11">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <v>5</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="H11" t="s">
+        <v>154</v>
+      </c>
+      <c r="I11" t="s">
+        <v>172</v>
+      </c>
+      <c r="J11" t="s">
+        <v>160</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="N11" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="O11" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q11">
+        <v>750</v>
+      </c>
+      <c r="R11">
+        <v>21</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="1"/>
+        <v>157.5</v>
+      </c>
+      <c r="U11">
+        <f>ROUND(Q11*T11/100,2)</f>
         <v>0</v>
       </c>
-      <c r="BM9">
-        <f t="shared" si="1"/>
-        <v>726.18</v>
-      </c>
-    </row>
-    <row r="10" spans="2:65" x14ac:dyDescent="0.15">
-      <c r="B10" s="9">
-        <v>45632</v>
-      </c>
-      <c r="C10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10">
-        <v>5</v>
-      </c>
-      <c r="E10" t="s">
-        <v>154</v>
-      </c>
-      <c r="F10" t="s">
-        <v>174</v>
-      </c>
-      <c r="G10">
-        <v>750</v>
-      </c>
-      <c r="H10">
-        <v>21</v>
-      </c>
-      <c r="I10">
+      <c r="X11">
         <f t="shared" si="2"/>
-        <v>157.5</v>
-      </c>
-      <c r="J10" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="K10">
-        <v>12</v>
-      </c>
-      <c r="L10" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="M10" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="N10" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>160</v>
-      </c>
-      <c r="R10" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="S10" s="10"/>
-      <c r="U10">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="X10">
+      <c r="Z11">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="Z10">
+      <c r="AC11">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AC10">
+      <c r="AE11">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AE10">
+      <c r="AH11">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AH10">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="BJ10">
+      <c r="BJ11">
         <v>750</v>
       </c>
-      <c r="BK10">
+      <c r="BK11">
         <v>19</v>
       </c>
-      <c r="BL10">
-        <f t="shared" ref="BL10" si="8">ROUND(BJ10*BK10/100,2)</f>
+      <c r="BL11">
+        <f t="shared" ref="BL11" si="7">ROUND(BJ11*BK11/100,2)</f>
         <v>142.5</v>
       </c>
-      <c r="BM10">
-        <f t="shared" si="1"/>
+      <c r="BM11">
+        <f>Q11+S11+U11+V11+X11+Z11+AA11+AC11+AE11+AF11+AH11+AJ11-BL11</f>
         <v>765</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="J2:K2"/>
+  <mergeCells count="9">
+    <mergeCell ref="BE3:BI3"/>
+    <mergeCell ref="AF3:AJ3"/>
+    <mergeCell ref="AK3:AO3"/>
+    <mergeCell ref="AP3:AT3"/>
+    <mergeCell ref="AU3:AY3"/>
+    <mergeCell ref="AZ3:BD3"/>
+    <mergeCell ref="Q3:U3"/>
+    <mergeCell ref="V3:Z3"/>
+    <mergeCell ref="AA3:AE3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Version v1.3.3.0 - Añadida clase 'Configuracion' para recoger los parametros pasados. - Añadido parametro 'HojaExcel' para permitir pasar el numero de hoja en la que estan los datos a importar - Modificados los metodos 'Procesos', 'ProcesoDiagram' y 'ProcesoAlcasal' para utilizar la clase 'Configuracion' - Añadido una lista de procesos validos que se chequea en el metodo 'ProcesarArgumentos' - Se añaden controles a los parametros pasados para evitar errores (genera fichero de errores.txt si alguno falla)
</commit_message>
<xml_diff>
--- a/pruebas/emitidasDiagram.xlsx
+++ b/pruebas/emitidasDiagram.xlsx
@@ -1055,9 +1055,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BM11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1950,7 +1948,7 @@
         <v>232.08</v>
       </c>
       <c r="U5">
-        <f>ROUND(Q5*T5/100,2)</f>
+        <f t="shared" ref="U5:U11" si="1">ROUND(Q5*T5/100,2)</f>
         <v>0</v>
       </c>
       <c r="V5">
@@ -1992,7 +1990,7 @@
         <v>0</v>
       </c>
       <c r="BM5">
-        <f>Q5+S5+U5+V5+X5+Z5+AA5+AC5+AE5+AF5+AH5+AJ5-BL5</f>
+        <f t="shared" ref="BM5:BM11" si="2">Q5+S5+U5+V5+X5+Z5+AA5+AC5+AE5+AF5+AH5+AJ5-BL5</f>
         <v>2710.42</v>
       </c>
     </row>
@@ -2041,11 +2039,11 @@
         <v>21</v>
       </c>
       <c r="S6">
-        <f t="shared" ref="S6:S11" si="1">ROUND(Q6*R6/100,2)</f>
+        <f t="shared" ref="S6:S11" si="3">ROUND(Q6*R6/100,2)</f>
         <v>84.15</v>
       </c>
       <c r="U6">
-        <f>ROUND(Q6*T6/100,2)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V6">
@@ -2055,11 +2053,11 @@
         <v>10</v>
       </c>
       <c r="X6">
-        <f t="shared" ref="X6:X11" si="2">ROUND(V6*W6/100,2)</f>
+        <f t="shared" ref="X6:X11" si="4">ROUND(V6*W6/100,2)</f>
         <v>34.57</v>
       </c>
       <c r="Z6">
-        <f t="shared" ref="Z6:Z11" si="3">ROUND(V6*Y6/100,2)</f>
+        <f t="shared" ref="Z6:Z11" si="5">ROUND(V6*Y6/100,2)</f>
         <v>0</v>
       </c>
       <c r="AA6">
@@ -2069,19 +2067,19 @@
         <v>4</v>
       </c>
       <c r="AC6">
-        <f t="shared" ref="AC6:AC11" si="4">ROUND(AA6*AB6/100,2)</f>
+        <f t="shared" ref="AC6:AC11" si="6">ROUND(AA6*AB6/100,2)</f>
         <v>12.41</v>
       </c>
       <c r="AE6">
-        <f t="shared" ref="AE6:AE11" si="5">ROUND(AA6*AD6/100,2)</f>
+        <f t="shared" ref="AE6:AE11" si="7">ROUND(AA6*AD6/100,2)</f>
         <v>0</v>
       </c>
       <c r="AH6">
-        <f t="shared" ref="AH6:AH11" si="6">ROUND(AF6*AG6/100,2)</f>
+        <f t="shared" ref="AH6:AH11" si="8">ROUND(AF6*AG6/100,2)</f>
         <v>0</v>
       </c>
       <c r="BM6">
-        <f>Q6+S6+U6+V6+X6+Z6+AA6+AC6+AE6+AF6+AH6+AJ6-BL6</f>
+        <f t="shared" si="2"/>
         <v>1187.8600000000001</v>
       </c>
     </row>
@@ -2130,11 +2128,11 @@
         <v>21</v>
       </c>
       <c r="S7">
+        <f t="shared" si="3"/>
+        <v>28.51</v>
+      </c>
+      <c r="U7">
         <f t="shared" si="1"/>
-        <v>28.51</v>
-      </c>
-      <c r="U7">
-        <f>ROUND(Q7*T7/100,2)</f>
         <v>0</v>
       </c>
       <c r="V7">
@@ -2144,27 +2142,27 @@
         <v>10</v>
       </c>
       <c r="X7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>15.01</v>
       </c>
       <c r="Z7">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AC7">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AE7">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AH7">
+      <c r="AC7">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="AE7">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AH7">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="BM7">
-        <f>Q7+S7+U7+V7+X7+Z7+AA7+AC7+AE7+AF7+AH7+AJ7-BL7</f>
+        <f t="shared" si="2"/>
         <v>329.40999999999997</v>
       </c>
     </row>
@@ -2213,14 +2211,14 @@
         <v>21</v>
       </c>
       <c r="S8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>483.03</v>
       </c>
       <c r="T8">
         <v>5.2</v>
       </c>
       <c r="U8">
-        <f>ROUND(Q8*T8/100,2)</f>
+        <f t="shared" si="1"/>
         <v>119.61</v>
       </c>
       <c r="V8">
@@ -2230,14 +2228,14 @@
         <v>10</v>
       </c>
       <c r="X8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>17.09</v>
       </c>
       <c r="Y8">
         <v>1.4</v>
       </c>
       <c r="Z8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.39</v>
       </c>
       <c r="AA8">
@@ -2247,22 +2245,22 @@
         <v>4</v>
       </c>
       <c r="AC8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.63</v>
       </c>
       <c r="AD8">
         <v>0.5</v>
       </c>
       <c r="AE8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.2</v>
       </c>
       <c r="AH8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="BM8">
-        <f>Q8+S8+U8+V8+X8+Z8+AA8+AC8+AE8+AF8+AH8+AJ8-BL8</f>
+        <f t="shared" si="2"/>
         <v>3135.7400000000002</v>
       </c>
     </row>
@@ -2311,14 +2309,14 @@
         <v>21</v>
       </c>
       <c r="S9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>232.7</v>
       </c>
       <c r="T9">
         <v>5.2</v>
       </c>
       <c r="U9">
-        <f>ROUND(Q9*T9/100,2)</f>
+        <f t="shared" si="1"/>
         <v>57.62</v>
       </c>
       <c r="V9">
@@ -2328,14 +2326,14 @@
         <v>10</v>
       </c>
       <c r="X9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>81.02</v>
       </c>
       <c r="Y9">
         <v>1.4</v>
       </c>
       <c r="Z9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>11.34</v>
       </c>
       <c r="AA9">
@@ -2345,22 +2343,22 @@
         <v>4</v>
       </c>
       <c r="AC9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.66</v>
       </c>
       <c r="AD9">
         <v>0.5</v>
       </c>
       <c r="AE9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.46</v>
       </c>
       <c r="AH9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="BM9">
-        <f>Q9+S9+U9+V9+X9+Z9+AA9+AC9+AE9+AF9+AH9+AJ9-BL9</f>
+        <f t="shared" si="2"/>
         <v>2396.62</v>
       </c>
     </row>
@@ -2409,35 +2407,35 @@
         <v>21</v>
       </c>
       <c r="S10">
+        <f t="shared" si="3"/>
+        <v>126.03</v>
+      </c>
+      <c r="U10">
         <f t="shared" si="1"/>
-        <v>126.03</v>
-      </c>
-      <c r="U10">
-        <f>ROUND(Q10*T10/100,2)</f>
         <v>0</v>
       </c>
       <c r="X10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Z10">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AC10">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AE10">
+      <c r="Z10">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AH10">
+      <c r="AC10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="AE10">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AH10">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="BM10">
-        <f>Q10+S10+U10+V10+X10+Z10+AA10+AC10+AE10+AF10+AH10+AJ10-BL10</f>
+        <f t="shared" si="2"/>
         <v>726.18</v>
       </c>
     </row>
@@ -2486,33 +2484,33 @@
         <v>21</v>
       </c>
       <c r="S11">
+        <f t="shared" si="3"/>
+        <v>157.5</v>
+      </c>
+      <c r="U11">
         <f t="shared" si="1"/>
-        <v>157.5</v>
-      </c>
-      <c r="U11">
-        <f>ROUND(Q11*T11/100,2)</f>
         <v>0</v>
       </c>
       <c r="X11">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Z11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AC11">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AE11">
+      <c r="Z11">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AH11">
+      <c r="AC11">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="AE11">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AH11">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="BJ11">
         <v>750</v>
       </c>
@@ -2520,25 +2518,25 @@
         <v>19</v>
       </c>
       <c r="BL11">
-        <f t="shared" ref="BL11" si="7">ROUND(BJ11*BK11/100,2)</f>
+        <f t="shared" ref="BL11" si="9">ROUND(BJ11*BK11/100,2)</f>
         <v>142.5</v>
       </c>
       <c r="BM11">
-        <f>Q11+S11+U11+V11+X11+Z11+AA11+AC11+AE11+AF11+AH11+AJ11-BL11</f>
+        <f t="shared" si="2"/>
         <v>765</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="Q3:U3"/>
+    <mergeCell ref="V3:Z3"/>
+    <mergeCell ref="AA3:AE3"/>
     <mergeCell ref="BE3:BI3"/>
     <mergeCell ref="AF3:AJ3"/>
     <mergeCell ref="AK3:AO3"/>
     <mergeCell ref="AP3:AT3"/>
     <mergeCell ref="AU3:AY3"/>
     <mergeCell ref="AZ3:BD3"/>
-    <mergeCell ref="Q3:U3"/>
-    <mergeCell ref="V3:Z3"/>
-    <mergeCell ref="AA3:AE3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Version 1.4.1.0 - Revision general de metodos, y añadidos comentarios al codigo - Realizadas pruebas con guion de facturas emitidas (Diagram y Alcasal) y facturas recibidas
</commit_message>
<xml_diff>
--- a/pruebas/emitidasDiagram.xlsx
+++ b/pruebas/emitidasDiagram.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="186">
   <si>
     <t>Columna</t>
   </si>
@@ -734,7 +734,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -764,6 +764,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1055,15 +1058,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BM11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="3" max="3" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.625" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="27.625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.625" bestFit="1" customWidth="1"/>
@@ -1387,197 +1393,265 @@
       </c>
     </row>
     <row r="2" spans="1:65" x14ac:dyDescent="0.15">
+      <c r="A2" s="11">
+        <f>COLUMN(A2)</f>
+        <v>1</v>
+      </c>
       <c r="B2" s="11">
-        <v>1</v>
+        <f t="shared" ref="B2:BM2" si="1">COLUMN(B2)</f>
+        <v>2</v>
       </c>
       <c r="C2" s="11">
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="D2" s="11">
-        <v>3</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="E2" s="11">
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
       <c r="F2" s="11">
-        <v>5</v>
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="G2" s="11">
-        <v>6</v>
+        <f t="shared" si="1"/>
+        <v>7</v>
       </c>
       <c r="H2" s="11">
-        <v>7</v>
+        <f t="shared" si="1"/>
+        <v>8</v>
       </c>
       <c r="I2" s="11">
-        <v>8</v>
+        <f t="shared" si="1"/>
+        <v>9</v>
       </c>
       <c r="J2" s="11">
-        <v>9</v>
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
       <c r="K2" s="11">
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>11</v>
       </c>
       <c r="L2" s="11">
-        <v>11</v>
+        <f t="shared" si="1"/>
+        <v>12</v>
       </c>
       <c r="M2" s="11">
-        <v>12</v>
+        <f t="shared" si="1"/>
+        <v>13</v>
       </c>
       <c r="N2" s="11">
-        <v>13</v>
+        <f t="shared" si="1"/>
+        <v>14</v>
       </c>
       <c r="O2" s="11">
-        <v>14</v>
+        <f t="shared" si="1"/>
+        <v>15</v>
       </c>
       <c r="P2" s="11">
-        <v>15</v>
+        <f t="shared" si="1"/>
+        <v>16</v>
       </c>
       <c r="Q2" s="11">
-        <v>16</v>
+        <f t="shared" si="1"/>
+        <v>17</v>
       </c>
       <c r="R2" s="11">
-        <v>17</v>
+        <f t="shared" si="1"/>
+        <v>18</v>
       </c>
       <c r="S2" s="11">
-        <v>18</v>
+        <f t="shared" si="1"/>
+        <v>19</v>
       </c>
       <c r="T2" s="11">
-        <v>19</v>
+        <f t="shared" si="1"/>
+        <v>20</v>
       </c>
       <c r="U2" s="11">
-        <v>20</v>
+        <f t="shared" si="1"/>
+        <v>21</v>
       </c>
       <c r="V2" s="11">
-        <v>21</v>
+        <f t="shared" si="1"/>
+        <v>22</v>
       </c>
       <c r="W2" s="11">
-        <v>22</v>
+        <f t="shared" si="1"/>
+        <v>23</v>
       </c>
       <c r="X2" s="11">
-        <v>23</v>
+        <f t="shared" si="1"/>
+        <v>24</v>
       </c>
       <c r="Y2" s="11">
-        <v>24</v>
+        <f t="shared" si="1"/>
+        <v>25</v>
       </c>
       <c r="Z2" s="11">
-        <v>25</v>
+        <f t="shared" si="1"/>
+        <v>26</v>
       </c>
       <c r="AA2" s="11">
-        <v>26</v>
+        <f t="shared" si="1"/>
+        <v>27</v>
       </c>
       <c r="AB2" s="11">
-        <v>27</v>
+        <f t="shared" si="1"/>
+        <v>28</v>
       </c>
       <c r="AC2" s="11">
-        <v>28</v>
+        <f t="shared" si="1"/>
+        <v>29</v>
       </c>
       <c r="AD2" s="11">
-        <v>29</v>
+        <f t="shared" si="1"/>
+        <v>30</v>
       </c>
       <c r="AE2" s="11">
-        <v>30</v>
+        <f t="shared" si="1"/>
+        <v>31</v>
       </c>
       <c r="AF2" s="11">
-        <v>31</v>
+        <f t="shared" si="1"/>
+        <v>32</v>
       </c>
       <c r="AG2" s="11">
-        <v>32</v>
+        <f t="shared" si="1"/>
+        <v>33</v>
       </c>
       <c r="AH2" s="11">
-        <v>33</v>
+        <f t="shared" si="1"/>
+        <v>34</v>
       </c>
       <c r="AI2" s="11">
-        <v>34</v>
+        <f t="shared" si="1"/>
+        <v>35</v>
       </c>
       <c r="AJ2" s="11">
-        <v>35</v>
+        <f t="shared" si="1"/>
+        <v>36</v>
       </c>
       <c r="AK2" s="11">
-        <v>36</v>
+        <f t="shared" si="1"/>
+        <v>37</v>
       </c>
       <c r="AL2" s="11">
-        <v>37</v>
+        <f t="shared" si="1"/>
+        <v>38</v>
       </c>
       <c r="AM2" s="11">
-        <v>38</v>
+        <f t="shared" si="1"/>
+        <v>39</v>
       </c>
       <c r="AN2" s="11">
-        <v>39</v>
+        <f t="shared" si="1"/>
+        <v>40</v>
       </c>
       <c r="AO2" s="11">
-        <v>40</v>
+        <f t="shared" si="1"/>
+        <v>41</v>
       </c>
       <c r="AP2" s="11">
-        <v>41</v>
+        <f t="shared" si="1"/>
+        <v>42</v>
       </c>
       <c r="AQ2" s="11">
-        <v>42</v>
+        <f t="shared" si="1"/>
+        <v>43</v>
       </c>
       <c r="AR2" s="11">
-        <v>43</v>
+        <f t="shared" si="1"/>
+        <v>44</v>
       </c>
       <c r="AS2" s="11">
-        <v>44</v>
+        <f t="shared" si="1"/>
+        <v>45</v>
       </c>
       <c r="AT2" s="11">
-        <v>45</v>
+        <f t="shared" si="1"/>
+        <v>46</v>
       </c>
       <c r="AU2" s="11">
-        <v>46</v>
+        <f t="shared" si="1"/>
+        <v>47</v>
       </c>
       <c r="AV2" s="11">
-        <v>47</v>
+        <f t="shared" si="1"/>
+        <v>48</v>
       </c>
       <c r="AW2" s="11">
-        <v>48</v>
+        <f t="shared" si="1"/>
+        <v>49</v>
       </c>
       <c r="AX2" s="11">
-        <v>49</v>
+        <f t="shared" si="1"/>
+        <v>50</v>
       </c>
       <c r="AY2" s="11">
-        <v>50</v>
+        <f t="shared" si="1"/>
+        <v>51</v>
       </c>
       <c r="AZ2" s="11">
-        <v>51</v>
+        <f t="shared" si="1"/>
+        <v>52</v>
       </c>
       <c r="BA2" s="11">
-        <v>52</v>
+        <f t="shared" si="1"/>
+        <v>53</v>
       </c>
       <c r="BB2" s="11">
-        <v>53</v>
+        <f t="shared" si="1"/>
+        <v>54</v>
       </c>
       <c r="BC2" s="11">
-        <v>54</v>
+        <f t="shared" si="1"/>
+        <v>55</v>
       </c>
       <c r="BD2" s="11">
-        <v>55</v>
+        <f t="shared" si="1"/>
+        <v>56</v>
       </c>
       <c r="BE2" s="11">
-        <v>56</v>
+        <f t="shared" si="1"/>
+        <v>57</v>
       </c>
       <c r="BF2" s="11">
-        <v>57</v>
+        <f t="shared" si="1"/>
+        <v>58</v>
       </c>
       <c r="BG2" s="11">
-        <v>58</v>
+        <f t="shared" si="1"/>
+        <v>59</v>
       </c>
       <c r="BH2" s="11">
-        <v>59</v>
+        <f t="shared" si="1"/>
+        <v>60</v>
       </c>
       <c r="BI2" s="11">
-        <v>60</v>
+        <f t="shared" si="1"/>
+        <v>61</v>
       </c>
       <c r="BJ2" s="11">
-        <v>61</v>
+        <f t="shared" si="1"/>
+        <v>62</v>
       </c>
       <c r="BK2" s="11">
-        <v>62</v>
+        <f t="shared" si="1"/>
+        <v>63</v>
       </c>
       <c r="BL2" s="11">
-        <v>63</v>
+        <f t="shared" si="1"/>
+        <v>64</v>
       </c>
       <c r="BM2" s="11">
-        <v>64</v>
+        <f t="shared" si="1"/>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:65" x14ac:dyDescent="0.15">
@@ -1585,7 +1659,7 @@
         <v>178</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>180</v>
@@ -1599,9 +1673,7 @@
       <c r="F3" s="13" t="s">
         <v>180</v>
       </c>
-      <c r="G3" s="13" t="s">
-        <v>180</v>
-      </c>
+      <c r="G3" s="14"/>
       <c r="H3" s="13" t="s">
         <v>179</v>
       </c>
@@ -1629,69 +1701,69 @@
       <c r="P3" s="13" t="s">
         <v>180</v>
       </c>
-      <c r="Q3" s="14" t="s">
+      <c r="Q3" s="15" t="s">
         <v>181</v>
       </c>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14"/>
-      <c r="T3" s="14"/>
-      <c r="U3" s="14"/>
-      <c r="V3" s="14" t="s">
+      <c r="R3" s="15"/>
+      <c r="S3" s="15"/>
+      <c r="T3" s="15"/>
+      <c r="U3" s="15"/>
+      <c r="V3" s="15" t="s">
         <v>182</v>
       </c>
-      <c r="W3" s="14"/>
-      <c r="X3" s="14"/>
-      <c r="Y3" s="14"/>
-      <c r="Z3" s="14"/>
-      <c r="AA3" s="14" t="s">
+      <c r="W3" s="15"/>
+      <c r="X3" s="15"/>
+      <c r="Y3" s="15"/>
+      <c r="Z3" s="15"/>
+      <c r="AA3" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="AB3" s="14"/>
-      <c r="AC3" s="14"/>
-      <c r="AD3" s="14"/>
-      <c r="AE3" s="14"/>
-      <c r="AF3" s="14" t="s">
+      <c r="AB3" s="15"/>
+      <c r="AC3" s="15"/>
+      <c r="AD3" s="15"/>
+      <c r="AE3" s="15"/>
+      <c r="AF3" s="15" t="s">
         <v>184</v>
       </c>
-      <c r="AG3" s="14"/>
-      <c r="AH3" s="14"/>
-      <c r="AI3" s="14"/>
-      <c r="AJ3" s="14"/>
-      <c r="AK3" s="15" t="s">
+      <c r="AG3" s="15"/>
+      <c r="AH3" s="15"/>
+      <c r="AI3" s="15"/>
+      <c r="AJ3" s="15"/>
+      <c r="AK3" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="AL3" s="15"/>
-      <c r="AM3" s="15"/>
-      <c r="AN3" s="15"/>
-      <c r="AO3" s="15"/>
-      <c r="AP3" s="15" t="s">
+      <c r="AL3" s="16"/>
+      <c r="AM3" s="16"/>
+      <c r="AN3" s="16"/>
+      <c r="AO3" s="16"/>
+      <c r="AP3" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="AQ3" s="15"/>
-      <c r="AR3" s="15"/>
-      <c r="AS3" s="15"/>
-      <c r="AT3" s="15"/>
-      <c r="AU3" s="15" t="s">
+      <c r="AQ3" s="16"/>
+      <c r="AR3" s="16"/>
+      <c r="AS3" s="16"/>
+      <c r="AT3" s="16"/>
+      <c r="AU3" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="AV3" s="15"/>
-      <c r="AW3" s="15"/>
-      <c r="AX3" s="15"/>
-      <c r="AY3" s="15"/>
-      <c r="AZ3" s="15" t="s">
+      <c r="AV3" s="16"/>
+      <c r="AW3" s="16"/>
+      <c r="AX3" s="16"/>
+      <c r="AY3" s="16"/>
+      <c r="AZ3" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="BA3" s="15"/>
-      <c r="BB3" s="15"/>
-      <c r="BC3" s="15"/>
-      <c r="BD3" s="15"/>
-      <c r="BE3" s="15" t="s">
+      <c r="BA3" s="16"/>
+      <c r="BB3" s="16"/>
+      <c r="BC3" s="16"/>
+      <c r="BD3" s="16"/>
+      <c r="BE3" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="BF3" s="15"/>
-      <c r="BG3" s="15"/>
-      <c r="BH3" s="15"/>
-      <c r="BI3" s="15"/>
+      <c r="BF3" s="16"/>
+      <c r="BG3" s="16"/>
+      <c r="BH3" s="16"/>
+      <c r="BI3" s="16"/>
       <c r="BJ3" t="s">
         <v>180</v>
       </c>
@@ -1707,22 +1779,22 @@
     </row>
     <row r="4" spans="1:65" x14ac:dyDescent="0.15">
       <c r="B4" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="G4" s="12" t="s">
         <v>5</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>143</v>
       </c>
       <c r="H4" s="12" t="s">
         <v>71</v>
@@ -1900,20 +1972,20 @@
       </c>
     </row>
     <row r="5" spans="1:65" x14ac:dyDescent="0.15">
-      <c r="B5" s="9">
+      <c r="C5">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="G5" s="9">
         <v>45627</v>
-      </c>
-      <c r="D5">
-        <v>12</v>
-      </c>
-      <c r="E5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>137</v>
       </c>
       <c r="H5" t="s">
         <v>154</v>
@@ -1948,7 +2020,7 @@
         <v>232.08</v>
       </c>
       <c r="U5">
-        <f t="shared" ref="U5:U11" si="1">ROUND(Q5*T5/100,2)</f>
+        <f t="shared" ref="U5:U11" si="2">ROUND(Q5*T5/100,2)</f>
         <v>0</v>
       </c>
       <c r="V5">
@@ -1990,25 +2062,25 @@
         <v>0</v>
       </c>
       <c r="BM5">
-        <f t="shared" ref="BM5:BM11" si="2">Q5+S5+U5+V5+X5+Z5+AA5+AC5+AE5+AF5+AH5+AJ5-BL5</f>
+        <f t="shared" ref="BM5:BM11" si="3">Q5+S5+U5+V5+X5+Z5+AA5+AC5+AE5+AF5+AH5+AJ5-BL5</f>
         <v>2710.42</v>
       </c>
     </row>
     <row r="6" spans="1:65" x14ac:dyDescent="0.15">
-      <c r="B6" s="9">
+      <c r="C6">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="G6" s="9">
         <v>45628</v>
-      </c>
-      <c r="D6">
-        <v>12</v>
-      </c>
-      <c r="E6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6">
-        <v>2</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>138</v>
       </c>
       <c r="H6" t="s">
         <v>155</v>
@@ -2039,11 +2111,11 @@
         <v>21</v>
       </c>
       <c r="S6">
-        <f t="shared" ref="S6:S11" si="3">ROUND(Q6*R6/100,2)</f>
+        <f t="shared" ref="S6:S11" si="4">ROUND(Q6*R6/100,2)</f>
         <v>84.15</v>
       </c>
       <c r="U6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="V6">
@@ -2053,11 +2125,11 @@
         <v>10</v>
       </c>
       <c r="X6">
-        <f t="shared" ref="X6:X11" si="4">ROUND(V6*W6/100,2)</f>
+        <f t="shared" ref="X6:X11" si="5">ROUND(V6*W6/100,2)</f>
         <v>34.57</v>
       </c>
       <c r="Z6">
-        <f t="shared" ref="Z6:Z11" si="5">ROUND(V6*Y6/100,2)</f>
+        <f t="shared" ref="Z6:Z11" si="6">ROUND(V6*Y6/100,2)</f>
         <v>0</v>
       </c>
       <c r="AA6">
@@ -2067,37 +2139,37 @@
         <v>4</v>
       </c>
       <c r="AC6">
-        <f t="shared" ref="AC6:AC11" si="6">ROUND(AA6*AB6/100,2)</f>
+        <f t="shared" ref="AC6:AC11" si="7">ROUND(AA6*AB6/100,2)</f>
         <v>12.41</v>
       </c>
       <c r="AE6">
-        <f t="shared" ref="AE6:AE11" si="7">ROUND(AA6*AD6/100,2)</f>
+        <f t="shared" ref="AE6:AE11" si="8">ROUND(AA6*AD6/100,2)</f>
         <v>0</v>
       </c>
       <c r="AH6">
-        <f t="shared" ref="AH6:AH11" si="8">ROUND(AF6*AG6/100,2)</f>
+        <f t="shared" ref="AH6:AH11" si="9">ROUND(AF6*AG6/100,2)</f>
         <v>0</v>
       </c>
       <c r="BM6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1187.8600000000001</v>
       </c>
     </row>
     <row r="7" spans="1:65" x14ac:dyDescent="0.15">
-      <c r="B7" s="9">
+      <c r="C7">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="G7" s="9">
         <v>45629</v>
-      </c>
-      <c r="D7">
-        <v>12</v>
-      </c>
-      <c r="E7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7">
-        <v>3</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>139</v>
       </c>
       <c r="H7" t="s">
         <v>157</v>
@@ -2128,11 +2200,11 @@
         <v>21</v>
       </c>
       <c r="S7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>28.51</v>
       </c>
       <c r="U7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="V7">
@@ -2142,45 +2214,45 @@
         <v>10</v>
       </c>
       <c r="X7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>15.01</v>
       </c>
       <c r="Z7">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="AC7">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AE7">
+      <c r="AC7">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AH7">
+      <c r="AE7">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
+      <c r="AH7">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
       <c r="BM7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>329.40999999999997</v>
       </c>
     </row>
     <row r="8" spans="1:65" x14ac:dyDescent="0.15">
-      <c r="B8" s="9">
+      <c r="C8">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="G8" s="9">
         <v>45630</v>
-      </c>
-      <c r="D8">
-        <v>12</v>
-      </c>
-      <c r="E8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>141</v>
       </c>
       <c r="H8" t="s">
         <v>156</v>
@@ -2211,14 +2283,14 @@
         <v>21</v>
       </c>
       <c r="S8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>483.03</v>
       </c>
       <c r="T8">
         <v>5.2</v>
       </c>
       <c r="U8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>119.61</v>
       </c>
       <c r="V8">
@@ -2228,14 +2300,14 @@
         <v>10</v>
       </c>
       <c r="X8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>17.09</v>
       </c>
       <c r="Y8">
         <v>1.4</v>
       </c>
       <c r="Z8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.39</v>
       </c>
       <c r="AA8">
@@ -2245,40 +2317,40 @@
         <v>4</v>
       </c>
       <c r="AC8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.63</v>
       </c>
       <c r="AD8">
         <v>0.5</v>
       </c>
       <c r="AE8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.2</v>
       </c>
       <c r="AH8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="BM8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3135.7400000000002</v>
       </c>
     </row>
     <row r="9" spans="1:65" x14ac:dyDescent="0.15">
-      <c r="B9" s="9">
+      <c r="C9">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="G9" s="9">
         <v>45630</v>
-      </c>
-      <c r="D9">
-        <v>12</v>
-      </c>
-      <c r="E9" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9">
-        <v>2</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>142</v>
       </c>
       <c r="H9" t="s">
         <v>159</v>
@@ -2309,14 +2381,14 @@
         <v>21</v>
       </c>
       <c r="S9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>232.7</v>
       </c>
       <c r="T9">
         <v>5.2</v>
       </c>
       <c r="U9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>57.62</v>
       </c>
       <c r="V9">
@@ -2326,14 +2398,14 @@
         <v>10</v>
       </c>
       <c r="X9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>81.02</v>
       </c>
       <c r="Y9">
         <v>1.4</v>
       </c>
       <c r="Z9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>11.34</v>
       </c>
       <c r="AA9">
@@ -2343,40 +2415,40 @@
         <v>4</v>
       </c>
       <c r="AC9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.66</v>
       </c>
       <c r="AD9">
         <v>0.5</v>
       </c>
       <c r="AE9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.46</v>
       </c>
       <c r="AH9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="BM9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2396.62</v>
       </c>
     </row>
     <row r="10" spans="1:65" x14ac:dyDescent="0.15">
-      <c r="B10" s="9">
+      <c r="C10">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="G10" s="9">
         <v>45631</v>
-      </c>
-      <c r="D10">
-        <v>12</v>
-      </c>
-      <c r="E10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10">
-        <v>4</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>150</v>
       </c>
       <c r="H10" t="s">
         <v>158</v>
@@ -2407,53 +2479,53 @@
         <v>21</v>
       </c>
       <c r="S10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>126.03</v>
       </c>
       <c r="U10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="X10">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Z10">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AC10">
+      <c r="Z10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AE10">
+      <c r="AC10">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AH10">
+      <c r="AE10">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
+      <c r="AH10">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
       <c r="BM10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>726.18</v>
       </c>
     </row>
     <row r="11" spans="1:65" x14ac:dyDescent="0.15">
-      <c r="B11" s="9">
+      <c r="C11">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="G11" s="9">
         <v>45632</v>
-      </c>
-      <c r="D11">
-        <v>12</v>
-      </c>
-      <c r="E11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F11">
-        <v>5</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>140</v>
       </c>
       <c r="H11" t="s">
         <v>154</v>
@@ -2484,33 +2556,33 @@
         <v>21</v>
       </c>
       <c r="S11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>157.5</v>
       </c>
       <c r="U11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="X11">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Z11">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AC11">
+      <c r="Z11">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AE11">
+      <c r="AC11">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AH11">
+      <c r="AE11">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
+      <c r="AH11">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
       <c r="BJ11">
         <v>750</v>
       </c>
@@ -2518,11 +2590,11 @@
         <v>19</v>
       </c>
       <c r="BL11">
-        <f t="shared" ref="BL11" si="9">ROUND(BJ11*BK11/100,2)</f>
+        <f t="shared" ref="BL11" si="10">ROUND(BJ11*BK11/100,2)</f>
         <v>142.5</v>
       </c>
       <c r="BM11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>765</v>
       </c>
     </row>

</xml_diff>